<commit_message>
code for simulations with fixed order and changed fake scenario rates
</commit_message>
<xml_diff>
--- a/Data/fake_calib.xlsx
+++ b/Data/fake_calib.xlsx
@@ -1944,85 +1944,85 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3340404348652283</v>
+        <v>0.3427596652611169</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3347079805834534</v>
+        <v>0.3541826681221227</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3347079805834534</v>
+        <v>0.3541826681221227</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3752346294103863</v>
+        <v>0.3268863512317419</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3922716252011579</v>
+        <v>0.4583146212155819</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3944772219934877</v>
+        <v>0.6541266520287885</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4600799632574016</v>
+        <v>0.8247938830593875</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2966012711958517</v>
+        <v>0.9371218080450195</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4358675197863172</v>
+        <v>0.9647509538584461</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6182669047624975</v>
+        <v>0.9873573481557857</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8513871523589532</v>
+        <v>0.9973130739359187</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9620427126226556</v>
+        <v>0.9979771939612142</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9860392888666988</v>
+        <v>0.9997814539076409</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9929078210859577</v>
+        <v>0.9999833322458218</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9992662735701949</v>
+        <v>0.9999970541461966</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.9998379075185956</v>
+        <v>0.9999995745640797</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9999645983815237</v>
+        <v>0.9999998008325693</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9999927514978374</v>
+        <v>0.9999999668526597</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9999992454839886</v>
+        <v>0.9999999985575037</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9999999614369973</v>
+        <v>0.9999999998144548</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9999999942334874</v>
+        <v>0.9999999999873046</v>
       </c>
       <c r="W2" t="n">
-        <v>0.9999999996984348</v>
+        <v>0.9999999999988014</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9999999999786235</v>
+        <v>0.9999999999999579</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.9999999999981554</v>
+        <v>0.9999999999999963</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.9999999999997964</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.9999999999999879</v>
+        <v>1</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.9999999999999983</v>
+        <v>1</v>
       </c>
       <c r="AC2" t="n">
         <v>1</v>
@@ -3451,547 +3451,547 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3340409153854845</v>
+        <v>0.3427662859909585</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3347089149296835</v>
+        <v>0.3541979297884076</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3347089149296835</v>
+        <v>0.3541979297884076</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3329975724132029</v>
+        <v>0.361111769631164</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3438018068010766</v>
+        <v>0.3403373519064756</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3707159967439892</v>
+        <v>0.2628976649311676</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3803926811126996</v>
+        <v>0.1537366801284825</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4921153619838561</v>
+        <v>0.05913263913741635</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4928919907493968</v>
+        <v>0.03468063821928633</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3609244536457368</v>
+        <v>0.01257263331736224</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1475289590451372</v>
+        <v>0.00268533981024382</v>
       </c>
       <c r="M3" t="n">
-        <v>0.03784186817292871</v>
+        <v>0.002022749992706098</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01394088429619788</v>
+        <v>0.0002185445744666497</v>
       </c>
       <c r="O3" t="n">
-        <v>0.007090673380250024</v>
+        <v>1.666773542600662e-05</v>
       </c>
       <c r="P3" t="n">
-        <v>0.00073366923636636</v>
+        <v>2.945852747921438e-06</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0001620877337326879</v>
+        <v>4.254358517423905e-07</v>
       </c>
       <c r="R3" t="n">
-        <v>3.540118140538131e-05</v>
+        <v>1.99167423632438e-07</v>
       </c>
       <c r="S3" t="n">
-        <v>7.248474833486213e-06</v>
+        <v>3.31473401019379e-08</v>
       </c>
       <c r="T3" t="n">
-        <v>7.545150987141433e-07</v>
+        <v>1.442496423777087e-09</v>
       </c>
       <c r="U3" t="n">
-        <v>3.856298618381731e-08</v>
+        <v>1.855452729428554e-10</v>
       </c>
       <c r="V3" t="n">
-        <v>5.766511761166752e-09</v>
+        <v>1.269541200584996e-11</v>
       </c>
       <c r="W3" t="n">
-        <v>3.015652413796354e-10</v>
+        <v>1.198599604389978e-12</v>
       </c>
       <c r="X3" t="n">
-        <v>2.137638985290491e-11</v>
+        <v>4.203488742283667e-14</v>
       </c>
       <c r="Y3" t="n">
-        <v>1.844665784313066e-12</v>
+        <v>3.755164089538632e-15</v>
       </c>
       <c r="Z3" t="n">
-        <v>2.035534666306683e-13</v>
+        <v>2.797379799038071e-16</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.214894822231783e-14</v>
+        <v>2.557007798978995e-17</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.666990526497639e-15</v>
+        <v>1.172572610229898e-18</v>
       </c>
       <c r="AC3" t="n">
-        <v>8.300786081448171e-17</v>
+        <v>6.603362247966267e-19</v>
       </c>
       <c r="AD3" t="n">
-        <v>5.977884164944131e-18</v>
+        <v>2.166833554182291e-20</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.650127603693046e-19</v>
+        <v>3.805837907946631e-22</v>
       </c>
       <c r="AF3" t="n">
-        <v>1.35394776181551e-20</v>
+        <v>8.372901686932888e-24</v>
       </c>
       <c r="AG3" t="n">
-        <v>5.426432652454927e-22</v>
+        <v>5.414391799579358e-25</v>
       </c>
       <c r="AH3" t="n">
-        <v>1.615171187877454e-23</v>
+        <v>2.828090799179087e-26</v>
       </c>
       <c r="AI3" t="n">
-        <v>8.989501213543593e-25</v>
+        <v>4.085326200738089e-28</v>
       </c>
       <c r="AJ3" t="n">
-        <v>2.868942098447846e-26</v>
+        <v>3.727988239942246e-29</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.933683579938293e-27</v>
+        <v>2.714277107721444e-30</v>
       </c>
       <c r="AL3" t="n">
-        <v>1.68028570394257e-28</v>
+        <v>5.264353403955752e-32</v>
       </c>
       <c r="AM3" t="n">
-        <v>1.042484665212469e-29</v>
+        <v>1.583891160722766e-33</v>
       </c>
       <c r="AN3" t="n">
-        <v>3.352275637611087e-31</v>
+        <v>2.748049144684999e-35</v>
       </c>
       <c r="AO3" t="n">
-        <v>9.720150435232676e-33</v>
+        <v>3.64044519694e-37</v>
       </c>
       <c r="AP3" t="n">
-        <v>4.535082485319513e-34</v>
+        <v>8.12845318118852e-39</v>
       </c>
       <c r="AQ3" t="n">
-        <v>5.438834835337646e-36</v>
+        <v>3.091192748687014e-40</v>
       </c>
       <c r="AR3" t="n">
-        <v>9.519622211263081e-38</v>
+        <v>3.224206795562875e-42</v>
       </c>
       <c r="AS3" t="n">
-        <v>3.115037959051576e-39</v>
+        <v>5.12738544660974e-44</v>
       </c>
       <c r="AT3" t="n">
-        <v>1.136400836907979e-40</v>
+        <v>3.883185230836167e-46</v>
       </c>
       <c r="AU3" t="n">
-        <v>6.078132564138721e-42</v>
+        <v>1.460975462026701e-48</v>
       </c>
       <c r="AV3" t="n">
-        <v>1.315405458496721e-43</v>
+        <v>8.803384327305877e-50</v>
       </c>
       <c r="AW3" t="n">
-        <v>3.175711166224074e-45</v>
+        <v>4.274060688115296e-53</v>
       </c>
       <c r="AX3" t="n">
-        <v>4.794707218417966e-46</v>
+        <v>2.569055580223472e-54</v>
       </c>
       <c r="AY3" t="n">
-        <v>1.757082244612227e-47</v>
+        <v>2.697471363059318e-56</v>
       </c>
       <c r="AZ3" t="n">
-        <v>3.455395372938413e-49</v>
+        <v>2.498160540392393e-58</v>
       </c>
       <c r="BA3" t="n">
-        <v>1.183191124374331e-50</v>
+        <v>5.725856124009929e-60</v>
       </c>
       <c r="BB3" t="n">
-        <v>2.171087701589236e-52</v>
+        <v>2.295796814516429e-62</v>
       </c>
       <c r="BC3" t="n">
-        <v>4.995145550529099e-54</v>
+        <v>7.424262716962657e-65</v>
       </c>
       <c r="BD3" t="n">
-        <v>1.350945558730478e-55</v>
+        <v>1.636481362426462e-66</v>
       </c>
       <c r="BE3" t="n">
-        <v>2.322571960426637e-57</v>
+        <v>1.130647920048672e-68</v>
       </c>
       <c r="BF3" t="n">
-        <v>2.634077758702788e-59</v>
+        <v>8.854433926584382e-71</v>
       </c>
       <c r="BG3" t="n">
-        <v>9.93826467490353e-61</v>
+        <v>1.754610508289229e-72</v>
       </c>
       <c r="BH3" t="n">
-        <v>3.343999021622318e-62</v>
+        <v>3.254900999124739e-74</v>
       </c>
       <c r="BI3" t="n">
-        <v>6.700835070318589e-64</v>
+        <v>1.750380598240082e-76</v>
       </c>
       <c r="BJ3" t="n">
-        <v>1.355427189042322e-65</v>
+        <v>9.450359807345318e-79</v>
       </c>
       <c r="BK3" t="n">
-        <v>1.680558359233124e-67</v>
+        <v>3.694434648236987e-80</v>
       </c>
       <c r="BL3" t="n">
-        <v>4.546941981469677e-69</v>
+        <v>3.516057092105157e-82</v>
       </c>
       <c r="BM3" t="n">
-        <v>7.695707070082521e-71</v>
+        <v>1.323257677941257e-84</v>
       </c>
       <c r="BN3" t="n">
-        <v>3.577306824474338e-72</v>
+        <v>1.892249600309881e-86</v>
       </c>
       <c r="BO3" t="n">
-        <v>5.195156191061356e-74</v>
+        <v>1.400094932950389e-88</v>
       </c>
       <c r="BP3" t="n">
-        <v>3.651197449833846e-76</v>
+        <v>5.206157046282093e-91</v>
       </c>
       <c r="BQ3" t="n">
-        <v>7.054548361506959e-78</v>
+        <v>2.682057716346431e-93</v>
       </c>
       <c r="BR3" t="n">
-        <v>2.017443894857068e-79</v>
+        <v>3.373519413952962e-95</v>
       </c>
       <c r="BS3" t="n">
-        <v>3.490658791994419e-81</v>
+        <v>1.181623136458306e-97</v>
       </c>
       <c r="BT3" t="n">
-        <v>7.795795242931761e-83</v>
+        <v>7.015090265235662e-100</v>
       </c>
       <c r="BU3" t="n">
-        <v>1.640382648354902e-84</v>
+        <v>2.918432085258258e-102</v>
       </c>
       <c r="BV3" t="n">
-        <v>2.759136204331163e-86</v>
+        <v>5.260428675582503e-105</v>
       </c>
       <c r="BW3" t="n">
-        <v>5.046766187517585e-88</v>
+        <v>2.897125849530734e-107</v>
       </c>
       <c r="BX3" t="n">
-        <v>5.78324201278763e-90</v>
+        <v>5.179033739009669e-109</v>
       </c>
       <c r="BY3" t="n">
-        <v>5.441971989194643e-92</v>
+        <v>1.984223654361901e-111</v>
       </c>
       <c r="BZ3" t="n">
-        <v>1.618506730649199e-93</v>
+        <v>4.07670403430276e-113</v>
       </c>
       <c r="CA3" t="n">
-        <v>1.497937468456311e-95</v>
+        <v>1.676901476684942e-115</v>
       </c>
       <c r="CB3" t="n">
-        <v>1.822452578959378e-97</v>
+        <v>4.26004298014749e-118</v>
       </c>
       <c r="CC3" t="n">
-        <v>1.896622094924564e-99</v>
+        <v>2.049205728627791e-120</v>
       </c>
       <c r="CD3" t="n">
-        <v>1.883644018091568e-101</v>
+        <v>1.87318107116676e-122</v>
       </c>
       <c r="CE3" t="n">
-        <v>2.890217391512314e-103</v>
+        <v>8.845138615869789e-125</v>
       </c>
       <c r="CF3" t="n">
-        <v>1.92708259410063e-105</v>
+        <v>6.140739203362763e-127</v>
       </c>
       <c r="CG3" t="n">
-        <v>2.195075687414651e-107</v>
+        <v>6.212339535281709e-129</v>
       </c>
       <c r="CH3" t="n">
-        <v>2.451454387089283e-109</v>
+        <v>2.850803642900186e-130</v>
       </c>
       <c r="CI3" t="n">
-        <v>3.710651016533665e-111</v>
+        <v>1.050737396927628e-132</v>
       </c>
       <c r="CJ3" t="n">
-        <v>9.668507985021522e-113</v>
+        <v>1.507429944073061e-135</v>
       </c>
       <c r="CK3" t="n">
-        <v>8.709759368055331e-115</v>
+        <v>3.940262170866269e-138</v>
       </c>
       <c r="CL3" t="n">
-        <v>6.146161677240962e-117</v>
+        <v>5.086084543020266e-140</v>
       </c>
       <c r="CM3" t="n">
-        <v>1.745852100284218e-118</v>
+        <v>3.637275792369754e-142</v>
       </c>
       <c r="CN3" t="n">
-        <v>2.18919372773414e-120</v>
+        <v>2.514792844802071e-144</v>
       </c>
       <c r="CO3" t="n">
-        <v>2.772482282626147e-122</v>
+        <v>4.700492641061687e-146</v>
       </c>
       <c r="CP3" t="n">
-        <v>4.377620872999403e-124</v>
+        <v>3.476353466527314e-148</v>
       </c>
       <c r="CQ3" t="n">
-        <v>7.857297148957112e-126</v>
+        <v>1.089187876949454e-150</v>
       </c>
       <c r="CR3" t="n">
-        <v>8.38851823328916e-128</v>
+        <v>1.083169531989692e-152</v>
       </c>
       <c r="CS3" t="n">
-        <v>1.481183240967473e-129</v>
+        <v>1.630582516716527e-155</v>
       </c>
       <c r="CT3" t="n">
-        <v>1.179899317320068e-131</v>
+        <v>9.761088090147579e-158</v>
       </c>
       <c r="CU3" t="n">
-        <v>8.14624300825685e-134</v>
+        <v>4.579237807792758e-160</v>
       </c>
       <c r="CV3" t="n">
-        <v>5.771648895100471e-136</v>
+        <v>2.765862080937066e-162</v>
       </c>
       <c r="CW3" t="n">
-        <v>8.300716943284907e-138</v>
+        <v>1.61476977632557e-164</v>
       </c>
       <c r="CX3" t="n">
-        <v>8.873148654829056e-140</v>
+        <v>6.472031680700426e-167</v>
       </c>
       <c r="CY3" t="n">
-        <v>1.735005764378078e-141</v>
+        <v>1.223186330154436e-169</v>
       </c>
       <c r="CZ3" t="n">
-        <v>2.009687638738139e-143</v>
+        <v>9.304217982964719e-172</v>
       </c>
       <c r="DA3" t="n">
-        <v>1.307441420760935e-145</v>
+        <v>5.982225501887548e-174</v>
       </c>
       <c r="DB3" t="n">
-        <v>9.910599581071714e-148</v>
+        <v>1.193425266845693e-175</v>
       </c>
       <c r="DC3" t="n">
-        <v>8.05031962974365e-150</v>
+        <v>3.967205672681683e-178</v>
       </c>
       <c r="DD3" t="n">
-        <v>9.764468497327537e-152</v>
+        <v>2.645127512227144e-180</v>
       </c>
       <c r="DE3" t="n">
-        <v>4.388155483487749e-153</v>
+        <v>1.635282915590281e-182</v>
       </c>
       <c r="DF3" t="n">
-        <v>3.500433596662767e-155</v>
+        <v>1.10326453468403e-184</v>
       </c>
       <c r="DG3" t="n">
-        <v>2.041200866160379e-157</v>
+        <v>2.429233097058146e-187</v>
       </c>
       <c r="DH3" t="n">
-        <v>2.266071614419807e-159</v>
+        <v>2.780871303097302e-190</v>
       </c>
       <c r="DI3" t="n">
-        <v>1.895005376929503e-161</v>
+        <v>6.89864438755543e-193</v>
       </c>
       <c r="DJ3" t="n">
-        <v>1.874981586751635e-163</v>
+        <v>3.965382250672598e-195</v>
       </c>
       <c r="DK3" t="n">
-        <v>1.017688909332548e-165</v>
+        <v>8.153752013387935e-198</v>
       </c>
       <c r="DL3" t="n">
-        <v>1.375755438919859e-167</v>
+        <v>1.700670078644917e-200</v>
       </c>
       <c r="DM3" t="n">
-        <v>9.597059096882656e-170</v>
+        <v>4.34546865097678e-203</v>
       </c>
       <c r="DN3" t="n">
-        <v>9.215520225958068e-172</v>
+        <v>9.61687350431176e-206</v>
       </c>
       <c r="DO3" t="n">
-        <v>5.932881977020188e-174</v>
+        <v>3.59902433832637e-208</v>
       </c>
       <c r="DP3" t="n">
-        <v>3.387217253787674e-176</v>
+        <v>6.679137998380817e-211</v>
       </c>
       <c r="DQ3" t="n">
-        <v>2.172067301277065e-178</v>
+        <v>4.15238950494621e-213</v>
       </c>
       <c r="DR3" t="n">
-        <v>1.819092172323801e-180</v>
+        <v>4.358027442567827e-215</v>
       </c>
       <c r="DS3" t="n">
-        <v>2.872735532658971e-182</v>
+        <v>1.474012048357474e-217</v>
       </c>
       <c r="DT3" t="n">
-        <v>1.832459560555893e-184</v>
+        <v>3.051490855830351e-220</v>
       </c>
       <c r="DU3" t="n">
-        <v>1.000818376344231e-186</v>
+        <v>1.101203248334439e-222</v>
       </c>
       <c r="DV3" t="n">
-        <v>8.045062306833243e-189</v>
+        <v>2.186051339006659e-225</v>
       </c>
       <c r="DW3" t="n">
-        <v>1.06906882180231e-190</v>
+        <v>1.346915123635053e-227</v>
       </c>
       <c r="DX3" t="n">
-        <v>5.990008641022124e-193</v>
+        <v>7.028862161712889e-230</v>
       </c>
       <c r="DY3" t="n">
-        <v>4.353441702241739e-195</v>
+        <v>1.690298489279362e-232</v>
       </c>
       <c r="DZ3" t="n">
-        <v>2.707894446077793e-197</v>
+        <v>2.938187694646752e-235</v>
       </c>
       <c r="EA3" t="n">
-        <v>1.450975068211758e-199</v>
+        <v>3.311946547586153e-237</v>
       </c>
       <c r="EB3" t="n">
-        <v>1.586334930695155e-201</v>
+        <v>4.714432392071598e-240</v>
       </c>
       <c r="EC3" t="n">
-        <v>1.100658655194018e-203</v>
+        <v>2.05673933053045e-242</v>
       </c>
       <c r="ED3" t="n">
-        <v>1.191272500860808e-205</v>
+        <v>7.359189334022428e-245</v>
       </c>
       <c r="EE3" t="n">
-        <v>7.39946785717612e-208</v>
+        <v>8.646399013395558e-247</v>
       </c>
       <c r="EF3" t="n">
-        <v>4.115887054752617e-210</v>
+        <v>5.898932705575344e-249</v>
       </c>
       <c r="EG3" t="n">
-        <v>3.944812136499779e-212</v>
+        <v>9.40705100328868e-252</v>
       </c>
       <c r="EH3" t="n">
-        <v>2.867985819228123e-214</v>
+        <v>1.937443718792838e-254</v>
       </c>
       <c r="EI3" t="n">
-        <v>5.758619839845654e-216</v>
+        <v>5.125000436502221e-257</v>
       </c>
       <c r="EJ3" t="n">
-        <v>4.203215045385939e-218</v>
+        <v>9.078024955783792e-260</v>
       </c>
       <c r="EK3" t="n">
-        <v>2.955015746378764e-220</v>
+        <v>2.689730561837005e-262</v>
       </c>
       <c r="EL3" t="n">
-        <v>1.635981271818948e-222</v>
+        <v>5.130364343944751e-265</v>
       </c>
       <c r="EM3" t="n">
-        <v>2.326014041612852e-224</v>
+        <v>8.980682407837718e-268</v>
       </c>
       <c r="EN3" t="n">
-        <v>1.160513096067633e-226</v>
+        <v>2.881607869200487e-270</v>
       </c>
       <c r="EO3" t="n">
-        <v>6.447166559235829e-229</v>
+        <v>5.509428102826226e-273</v>
       </c>
       <c r="EP3" t="n">
-        <v>3.501008108236934e-231</v>
+        <v>1.181455053778399e-275</v>
       </c>
       <c r="EQ3" t="n">
-        <v>2.197575538315502e-233</v>
+        <v>3.408811336360903e-278</v>
       </c>
       <c r="ER3" t="n">
-        <v>2.511286342262438e-235</v>
+        <v>1.170885495152195e-280</v>
       </c>
       <c r="ES3" t="n">
-        <v>3.36544087512229e-237</v>
+        <v>2.214856853139357e-283</v>
       </c>
       <c r="ET3" t="n">
-        <v>3.048391501840981e-239</v>
+        <v>1.807342929163372e-286</v>
       </c>
       <c r="EU3" t="n">
-        <v>1.371785094836016e-241</v>
+        <v>2.923337752566251e-289</v>
       </c>
       <c r="EV3" t="n">
-        <v>7.694714209327436e-244</v>
+        <v>2.271152685790388e-291</v>
       </c>
       <c r="EW3" t="n">
-        <v>3.82529391642505e-246</v>
+        <v>1.434105495617841e-293</v>
       </c>
       <c r="EX3" t="n">
-        <v>2.110968893164375e-248</v>
+        <v>4.340315144098762e-296</v>
       </c>
       <c r="EY3" t="n">
-        <v>1.233914067369514e-250</v>
+        <v>1.342419879775061e-298</v>
       </c>
       <c r="EZ3" t="n">
-        <v>3.220977073896067e-252</v>
+        <v>7.524255822441611e-301</v>
       </c>
       <c r="FA3" t="n">
-        <v>2.443686007743366e-254</v>
+        <v>2.375228166840238e-303</v>
       </c>
       <c r="FB3" t="n">
-        <v>1.042463050936734e-256</v>
+        <v>2.780794993952361e-306</v>
       </c>
       <c r="FC3" t="n">
-        <v>1.012956232674368e-258</v>
+        <v>0</v>
       </c>
       <c r="FD3" t="n">
-        <v>7.258495828264275e-261</v>
+        <v>0</v>
       </c>
       <c r="FE3" t="n">
-        <v>5.703455710982697e-263</v>
+        <v>0</v>
       </c>
       <c r="FF3" t="n">
-        <v>4.484757501229814e-265</v>
+        <v>0</v>
       </c>
       <c r="FG3" t="n">
-        <v>3.675050387552202e-267</v>
+        <v>0</v>
       </c>
       <c r="FH3" t="n">
-        <v>6.182593424994078e-269</v>
+        <v>0</v>
       </c>
       <c r="FI3" t="n">
-        <v>3.403723183903058e-271</v>
+        <v>0</v>
       </c>
       <c r="FJ3" t="n">
-        <v>8.974189545404788e-273</v>
+        <v>0</v>
       </c>
       <c r="FK3" t="n">
-        <v>7.219948224287143e-275</v>
+        <v>0</v>
       </c>
       <c r="FL3" t="n">
-        <v>3.453509830768677e-277</v>
+        <v>0</v>
       </c>
       <c r="FM3" t="n">
-        <v>2.101621655336595e-279</v>
+        <v>0</v>
       </c>
       <c r="FN3" t="n">
-        <v>1.13587174376456e-281</v>
+        <v>0</v>
       </c>
       <c r="FO3" t="n">
-        <v>5.832231174433887e-284</v>
+        <v>0</v>
       </c>
       <c r="FP3" t="n">
-        <v>2.429724647023535e-286</v>
+        <v>0</v>
       </c>
       <c r="FQ3" t="n">
-        <v>1.603364492935893e-288</v>
+        <v>0</v>
       </c>
       <c r="FR3" t="n">
-        <v>7.741670772150132e-291</v>
+        <v>0</v>
       </c>
       <c r="FS3" t="n">
-        <v>3.132259442085045e-293</v>
+        <v>0</v>
       </c>
       <c r="FT3" t="n">
-        <v>1.222214879478931e-295</v>
+        <v>0</v>
       </c>
       <c r="FU3" t="n">
-        <v>1.494363833108065e-297</v>
+        <v>0</v>
       </c>
       <c r="FV3" t="n">
-        <v>1.9671738314379e-299</v>
+        <v>0</v>
       </c>
       <c r="FW3" t="n">
-        <v>8.603032717706724e-302</v>
+        <v>0</v>
       </c>
       <c r="FX3" t="n">
-        <v>6.868087259528674e-304</v>
+        <v>0</v>
       </c>
       <c r="FY3" t="n">
-        <v>4.238582920990973e-306</v>
+        <v>0</v>
       </c>
       <c r="FZ3" t="n">
-        <v>2.175374895568657e-308</v>
+        <v>0</v>
       </c>
       <c r="GA3" t="n">
         <v>0</v>
@@ -4958,472 +4958,472 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3319186497492871</v>
+        <v>0.3144740487479245</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3305831044868631</v>
+        <v>0.2916194020894697</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3305831044868631</v>
+        <v>0.2916194020894697</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2917677981764108</v>
+        <v>0.3120018791370941</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2639265679977655</v>
+        <v>0.2013480268779424</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2348067812625229</v>
+        <v>0.08297568304004391</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1595273556298988</v>
+        <v>0.02146943681213007</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2112833668202923</v>
+        <v>0.003745552817564052</v>
       </c>
       <c r="J4" t="n">
-        <v>0.07124048946428613</v>
+        <v>0.0005684079222674549</v>
       </c>
       <c r="K4" t="n">
-        <v>0.02080864159176593</v>
+        <v>7.001852685207482e-05</v>
       </c>
       <c r="L4" t="n">
-        <v>0.001083888595909505</v>
+        <v>1.586253837566144e-06</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0001154192044158172</v>
+        <v>5.604607973673408e-08</v>
       </c>
       <c r="N4" t="n">
-        <v>1.982683710329176e-05</v>
+        <v>1.517892320096e-09</v>
       </c>
       <c r="O4" t="n">
-        <v>1.505533792377479e-06</v>
+        <v>1.875228437165671e-11</v>
       </c>
       <c r="P4" t="n">
-        <v>5.719343872046943e-08</v>
+        <v>1.055606727574964e-12</v>
       </c>
       <c r="Q4" t="n">
-        <v>4.74767168591162e-09</v>
+        <v>6.86144056121543e-14</v>
       </c>
       <c r="R4" t="n">
-        <v>4.370710031544406e-10</v>
+        <v>6.940838336370183e-15</v>
       </c>
       <c r="S4" t="n">
-        <v>2.732912985384216e-11</v>
+        <v>2.515492248722714e-16</v>
       </c>
       <c r="T4" t="n">
-        <v>9.126814953851872e-13</v>
+        <v>2.73135636534312e-18</v>
       </c>
       <c r="U4" t="n">
-        <v>1.647704468495585e-14</v>
+        <v>1.561995048723582e-19</v>
       </c>
       <c r="V4" t="n">
-        <v>7.406607629469932e-16</v>
+        <v>2.529515572748004e-21</v>
       </c>
       <c r="W4" t="n">
-        <v>1.230256447304669e-17</v>
+        <v>7.613108815774401e-23</v>
       </c>
       <c r="X4" t="n">
-        <v>3.360123050190351e-19</v>
+        <v>7.12565710632934e-25</v>
       </c>
       <c r="Y4" t="n">
-        <v>7.187771503984678e-21</v>
+        <v>1.379565034299684e-26</v>
       </c>
       <c r="Z4" t="n">
-        <v>2.524029664648558e-22</v>
+        <v>3.523040706237051e-28</v>
       </c>
       <c r="AA4" t="n">
-        <v>5.227086456128274e-24</v>
+        <v>6.659516049095996e-30</v>
       </c>
       <c r="AB4" t="n">
-        <v>2.761706152476095e-25</v>
+        <v>8.604668686227232e-32</v>
       </c>
       <c r="AC4" t="n">
-        <v>5.330147431639871e-27</v>
+        <v>7.881521112848575e-33</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.047670038770415e-28</v>
+        <v>9.975368742535246e-35</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.530272165925193e-30</v>
+        <v>5.474364969363437e-37</v>
       </c>
       <c r="AF4" t="n">
-        <v>4.370808150674366e-32</v>
+        <v>3.427274602337268e-39</v>
       </c>
       <c r="AG4" t="n">
-        <v>9.141228041402538e-34</v>
+        <v>4.929048293653462e-41</v>
       </c>
       <c r="AH4" t="n">
-        <v>1.089042723077547e-35</v>
+        <v>6.08881210238278e-43</v>
       </c>
       <c r="AI4" t="n">
-        <v>2.491291892970613e-37</v>
+        <v>4.618924965429883e-45</v>
       </c>
       <c r="AJ4" t="n">
-        <v>3.018530586415613e-39</v>
+        <v>1.422174510990053e-46</v>
       </c>
       <c r="AK4" t="n">
-        <v>9.483876312795798e-41</v>
+        <v>2.395844290301876e-48</v>
       </c>
       <c r="AL4" t="n">
-        <v>2.373640495668625e-42</v>
+        <v>1.513649543089383e-50</v>
       </c>
       <c r="AM4" t="n">
-        <v>4.535379319598907e-44</v>
+        <v>1.465677716599517e-52</v>
       </c>
       <c r="AN4" t="n">
-        <v>5.78120780738471e-46</v>
+        <v>7.899576257126463e-55</v>
       </c>
       <c r="AO4" t="n">
-        <v>6.529936229163554e-48</v>
+        <v>3.580894894287045e-57</v>
       </c>
       <c r="AP4" t="n">
-        <v>1.190726293711805e-49</v>
+        <v>2.569471110361318e-59</v>
       </c>
       <c r="AQ4" t="n">
-        <v>8.35044210219939e-52</v>
+        <v>2.849715854319165e-61</v>
       </c>
       <c r="AR4" t="n">
-        <v>8.15264782925545e-54</v>
+        <v>1.332672646576329e-63</v>
       </c>
       <c r="AS4" t="n">
-        <v>1.105708122529608e-55</v>
+        <v>6.879827731971005e-66</v>
       </c>
       <c r="AT4" t="n">
-        <v>1.42409400973381e-57</v>
+        <v>2.893914941178841e-68</v>
       </c>
       <c r="AU4" t="n">
-        <v>2.686893576639597e-59</v>
+        <v>6.644265996503585e-71</v>
       </c>
       <c r="AV4" t="n">
-        <v>2.484892665313006e-61</v>
+        <v>2.361866078620657e-72</v>
       </c>
       <c r="AW4" t="n">
-        <v>2.369712586001159e-63</v>
+        <v>2.648863140372622e-75</v>
       </c>
       <c r="AX4" t="n">
-        <v>1.03398953072773e-64</v>
+        <v>5.197947047778949e-77</v>
       </c>
       <c r="AY4" t="n">
-        <v>1.475388418844682e-66</v>
+        <v>3.193345265445578e-79</v>
       </c>
       <c r="AZ4" t="n">
-        <v>1.292772616923317e-68</v>
+        <v>1.207246095542122e-81</v>
       </c>
       <c r="BA4" t="n">
-        <v>1.827490442748944e-70</v>
+        <v>8.516860783852063e-84</v>
       </c>
       <c r="BB4" t="n">
-        <v>1.435891627265607e-72</v>
+        <v>1.958605929516812e-86</v>
       </c>
       <c r="BC4" t="n">
-        <v>1.3455359996558e-74</v>
+        <v>3.807585572739344e-89</v>
       </c>
       <c r="BD4" t="n">
-        <v>1.697849726502359e-76</v>
+        <v>2.972170068178993e-91</v>
       </c>
       <c r="BE4" t="n">
-        <v>1.267072145019762e-78</v>
+        <v>8.392891311218572e-94</v>
       </c>
       <c r="BF4" t="n">
-        <v>8.805788815150822e-81</v>
+        <v>2.871656237474261e-96</v>
       </c>
       <c r="BG4" t="n">
-        <v>1.139228470030571e-82</v>
+        <v>1.739066107648408e-98</v>
       </c>
       <c r="BH4" t="n">
-        <v>1.39492596060824e-84</v>
+        <v>1.085132317429354e-100</v>
       </c>
       <c r="BI4" t="n">
-        <v>1.596520997785556e-86</v>
+        <v>2.487868900138083e-103</v>
       </c>
       <c r="BJ4" t="n">
-        <v>1.280668032597698e-88</v>
+        <v>8.247123430947612e-106</v>
       </c>
       <c r="BK4" t="n">
-        <v>8.367121727857479e-91</v>
+        <v>8.414664092318983e-108</v>
       </c>
       <c r="BL4" t="n">
-        <v>1.08326314728504e-92</v>
+        <v>5.393968613809783e-110</v>
       </c>
       <c r="BM4" t="n">
-        <v>9.106372461080086e-95</v>
+        <v>1.831572047843212e-112</v>
       </c>
       <c r="BN4" t="n">
-        <v>2.156920479545289e-96</v>
+        <v>8.406161292740895e-115</v>
       </c>
       <c r="BO4" t="n">
-        <v>1.532336970615782e-98</v>
+        <v>2.871412782710483e-117</v>
       </c>
       <c r="BP4" t="n">
-        <v>7.273143245610504e-101</v>
+        <v>5.322894022927111e-120</v>
       </c>
       <c r="BQ4" t="n">
-        <v>6.351597868184872e-103</v>
+        <v>1.160605582457897e-122</v>
       </c>
       <c r="BR4" t="n">
-        <v>7.515240962520226e-105</v>
+        <v>5.227996431301397e-125</v>
       </c>
       <c r="BS4" t="n">
-        <v>5.287556161759059e-107</v>
+        <v>9.867340435726262e-128</v>
       </c>
       <c r="BT4" t="n">
-        <v>5.023219652289095e-109</v>
+        <v>2.340398227504519e-130</v>
       </c>
       <c r="BU4" t="n">
-        <v>4.033634978011259e-111</v>
+        <v>4.443087345050726e-133</v>
       </c>
       <c r="BV4" t="n">
-        <v>3.312769293316554e-113</v>
+        <v>5.870358806526632e-136</v>
       </c>
       <c r="BW4" t="n">
-        <v>2.716277716233866e-115</v>
+        <v>1.603363728808177e-138</v>
       </c>
       <c r="BX4" t="n">
-        <v>1.572422284378813e-117</v>
+        <v>1.240426598206409e-140</v>
       </c>
       <c r="BY4" t="n">
-        <v>7.544239294839086e-120</v>
+        <v>2.165415094790846e-143</v>
       </c>
       <c r="BZ4" t="n">
-        <v>1.106657272670346e-121</v>
+        <v>1.62542490720555e-145</v>
       </c>
       <c r="CA4" t="n">
-        <v>5.912972781466022e-124</v>
+        <v>2.907925236906733e-148</v>
       </c>
       <c r="CB4" t="n">
-        <v>3.347518502546232e-126</v>
+        <v>4.347221826765239e-151</v>
       </c>
       <c r="CC4" t="n">
-        <v>1.63818300863509e-128</v>
+        <v>8.550108605960992e-154</v>
       </c>
       <c r="CD4" t="n">
-        <v>8.192252156250613e-131</v>
+        <v>2.623876812190019e-156</v>
       </c>
       <c r="CE4" t="n">
-        <v>7.421859044097584e-133</v>
+        <v>5.013443310847943e-159</v>
       </c>
       <c r="CF4" t="n">
-        <v>3.014164327638837e-135</v>
+        <v>1.254535782824079e-161</v>
       </c>
       <c r="CG4" t="n">
-        <v>1.581816550888218e-137</v>
+        <v>4.308653815373942e-164</v>
       </c>
       <c r="CH4" t="n">
-        <v>8.244558171230561e-140</v>
+        <v>1.337864909472172e-165</v>
       </c>
       <c r="CI4" t="n">
-        <v>7.651683157547676e-142</v>
+        <v>2.228296391640593e-168</v>
       </c>
       <c r="CJ4" t="n">
-        <v>7.919687642235974e-144</v>
+        <v>2.985775307158822e-171</v>
       </c>
       <c r="CK4" t="n">
-        <v>3.60260635260251e-146</v>
+        <v>4.177224844496176e-174</v>
       </c>
       <c r="CL4" t="n">
-        <v>1.413581239051552e-148</v>
+        <v>1.970961214600416e-176</v>
       </c>
       <c r="CM4" t="n">
-        <v>1.922176049560373e-150</v>
+        <v>5.060017747821056e-179</v>
       </c>
       <c r="CN4" t="n">
-        <v>1.108698171730576e-152</v>
+        <v>1.338817221387493e-181</v>
       </c>
       <c r="CO4" t="n">
-        <v>6.146060188567437e-155</v>
+        <v>8.99632257440181e-184</v>
       </c>
       <c r="CP4" t="n">
-        <v>3.978205866488861e-157</v>
+        <v>2.341286652084689e-186</v>
       </c>
       <c r="CQ4" t="n">
-        <v>2.933743591334841e-159</v>
+        <v>3.62250959268338e-189</v>
       </c>
       <c r="CR4" t="n">
-        <v>1.507756257218197e-161</v>
+        <v>1.23343907073315e-191</v>
       </c>
       <c r="CS4" t="n">
-        <v>1.34543894324811e-163</v>
+        <v>1.338104491369608e-194</v>
       </c>
       <c r="CT4" t="n">
-        <v>5.464155663824618e-166</v>
+        <v>3.189812634516567e-197</v>
       </c>
       <c r="CU4" t="n">
-        <v>2.035578565099147e-168</v>
+        <v>6.615429908556727e-200</v>
       </c>
       <c r="CV4" t="n">
-        <v>7.832857215765465e-171</v>
+        <v>1.944451508502353e-202</v>
       </c>
       <c r="CW4" t="n">
-        <v>4.901006499599e-173</v>
+        <v>4.773899365744932e-205</v>
       </c>
       <c r="CX4" t="n">
-        <v>2.440297382399967e-175</v>
+        <v>1.033315207927565e-207</v>
       </c>
       <c r="CY4" t="n">
-        <v>2.669263871292161e-177</v>
+        <v>1.232609835109404e-210</v>
       </c>
       <c r="CZ4" t="n">
-        <v>1.617802964844949e-179</v>
+        <v>3.19972733572719e-213</v>
       </c>
       <c r="DA4" t="n">
-        <v>5.698757686110416e-182</v>
+        <v>7.386121688043113e-216</v>
       </c>
       <c r="DB4" t="n">
-        <v>2.30103166101287e-184</v>
+        <v>5.459012340844389e-218</v>
       </c>
       <c r="DC4" t="n">
-        <v>8.798198845475916e-187</v>
+        <v>1.222605265144879e-220</v>
       </c>
       <c r="DD4" t="n">
-        <v>4.750400388227549e-189</v>
+        <v>3.925703973492464e-223</v>
       </c>
       <c r="DE4" t="n">
-        <v>8.378183321268247e-191</v>
+        <v>1.154305659518337e-225</v>
       </c>
       <c r="DF4" t="n">
-        <v>3.114795290181529e-193</v>
+        <v>3.940433156338325e-228</v>
       </c>
       <c r="DG4" t="n">
-        <v>1.007176076699677e-195</v>
+        <v>4.38923578540947e-231</v>
       </c>
       <c r="DH4" t="n">
-        <v>6.476009757550537e-198</v>
+        <v>5.150023977981833e-234</v>
       </c>
       <c r="DI4" t="n">
-        <v>2.716775088533787e-200</v>
+        <v>7.392584284988975e-237</v>
       </c>
       <c r="DJ4" t="n">
-        <v>1.161945766869872e-202</v>
+        <v>1.543783410666238e-239</v>
       </c>
       <c r="DK4" t="n">
-        <v>3.765179905503862e-205</v>
+        <v>1.717143235919029e-242</v>
       </c>
       <c r="DL4" t="n">
-        <v>2.028084718570047e-207</v>
+        <v>1.822579441631194e-245</v>
       </c>
       <c r="DM4" t="n">
-        <v>7.672963995997875e-210</v>
+        <v>2.123365517965318e-248</v>
       </c>
       <c r="DN4" t="n">
-        <v>3.51694386336655e-212</v>
+        <v>2.277498903119555e-251</v>
       </c>
       <c r="DO4" t="n">
-        <v>1.171833681974876e-214</v>
+        <v>4.122880437484137e-254</v>
       </c>
       <c r="DP4" t="n">
-        <v>3.559877788501531e-217</v>
+        <v>4.405473239143327e-257</v>
       </c>
       <c r="DQ4" t="n">
-        <v>1.201441084848339e-219</v>
+        <v>1.271101304879624e-259</v>
       </c>
       <c r="DR4" t="n">
-        <v>4.653411922993553e-222</v>
+        <v>5.07494325981208e-262</v>
       </c>
       <c r="DS4" t="n">
-        <v>3.76709744347641e-224</v>
+        <v>7.051447467231932e-265</v>
       </c>
       <c r="DT4" t="n">
-        <v>1.175251836606625e-226</v>
+        <v>7.199613541457608e-268</v>
       </c>
       <c r="DU4" t="n">
-        <v>3.440918280775386e-229</v>
+        <v>1.109386814709119e-270</v>
       </c>
       <c r="DV4" t="n">
-        <v>1.298318655736247e-231</v>
+        <v>1.354899585665585e-273</v>
       </c>
       <c r="DW4" t="n">
-        <v>7.449357396518698e-234</v>
+        <v>3.902257686812246e-276</v>
       </c>
       <c r="DX4" t="n">
-        <v>2.188483646771313e-236</v>
+        <v>1.040739900855277e-278</v>
       </c>
       <c r="DY4" t="n">
-        <v>9.362464241152791e-239</v>
+        <v>1.201775876346571e-281</v>
       </c>
       <c r="DZ4" t="n">
-        <v>2.959273603858738e-241</v>
+        <v>1.156872723369773e-284</v>
       </c>
       <c r="EA4" t="n">
-        <v>8.599591142215919e-244</v>
+        <v>9.419491767105319e-287</v>
       </c>
       <c r="EB4" t="n">
-        <v>4.223423457859357e-246</v>
+        <v>9.200538294005018e-290</v>
       </c>
       <c r="EC4" t="n">
-        <v>1.463806514572832e-248</v>
+        <v>1.68886083007428e-292</v>
       </c>
       <c r="ED4" t="n">
-        <v>6.98546692302201e-251</v>
+        <v>2.646834406822808e-295</v>
       </c>
       <c r="EE4" t="n">
-        <v>2.059605793217707e-253</v>
+        <v>1.206690055092647e-297</v>
       </c>
       <c r="EF4" t="n">
-        <v>6.644158090819675e-256</v>
+        <v>4.023611816757313e-300</v>
       </c>
       <c r="EG4" t="n">
-        <v>2.835645498546618e-258</v>
+        <v>4.017310746149953e-303</v>
       </c>
       <c r="EH4" t="n">
-        <v>1.016398156819427e-260</v>
+        <v>4.331950816500556e-306</v>
       </c>
       <c r="EI4" t="n">
-        <v>1.187639877521587e-262</v>
+        <v>0</v>
       </c>
       <c r="EJ4" t="n">
-        <v>4.200214120435024e-265</v>
+        <v>0</v>
       </c>
       <c r="EK4" t="n">
-        <v>1.555540713567495e-267</v>
+        <v>0</v>
       </c>
       <c r="EL4" t="n">
-        <v>4.285008872579461e-270</v>
+        <v>0</v>
       </c>
       <c r="EM4" t="n">
-        <v>2.984314031978609e-272</v>
+        <v>0</v>
       </c>
       <c r="EN4" t="n">
-        <v>7.996010005852495e-275</v>
+        <v>0</v>
       </c>
       <c r="EO4" t="n">
-        <v>2.147293743386611e-277</v>
+        <v>0</v>
       </c>
       <c r="EP4" t="n">
-        <v>5.910503328153842e-280</v>
+        <v>0</v>
       </c>
       <c r="EQ4" t="n">
-        <v>1.757896745602168e-282</v>
+        <v>0</v>
       </c>
       <c r="ER4" t="n">
-        <v>1.001066900760418e-284</v>
+        <v>0</v>
       </c>
       <c r="ES4" t="n">
-        <v>6.813535103476538e-287</v>
+        <v>0</v>
       </c>
       <c r="ET4" t="n">
-        <v>3.195727187171522e-289</v>
+        <v>0</v>
       </c>
       <c r="EU4" t="n">
-        <v>7.890541854658281e-292</v>
+        <v>0</v>
       </c>
       <c r="EV4" t="n">
-        <v>2.094592833880953e-294</v>
+        <v>0</v>
       </c>
       <c r="EW4" t="n">
-        <v>5.249162276199452e-297</v>
+        <v>0</v>
       </c>
       <c r="EX4" t="n">
-        <v>1.420531682930035e-299</v>
+        <v>0</v>
       </c>
       <c r="EY4" t="n">
-        <v>4.262033246991208e-302</v>
+        <v>0</v>
       </c>
       <c r="EZ4" t="n">
-        <v>5.731179639679239e-304</v>
+        <v>0</v>
       </c>
       <c r="FA4" t="n">
-        <v>2.165679610363399e-306</v>
+        <v>0</v>
       </c>
       <c r="FB4" t="n">
         <v>0</v>
@@ -7986,547 +7986,547 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3342431986444114</v>
+        <v>0.3424440652432213</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3354185530979053</v>
+        <v>0.3209566884471627</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3354185530979053</v>
+        <v>0.3209566884471627</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3675963298281454</v>
+        <v>0.2310547208558697</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3437383607568873</v>
+        <v>0.3021008025738641</v>
       </c>
       <c r="G2" t="n">
-        <v>0.441090865585555</v>
+        <v>0.07281143196576603</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3921075253973714</v>
+        <v>0.09658504194260989</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4204174136217197</v>
+        <v>0.02274890698281252</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4486279711049425</v>
+        <v>0.006538666243121605</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2003779818360614</v>
+        <v>0.04547011694615025</v>
       </c>
       <c r="L2" t="n">
-        <v>0.152612826108953</v>
+        <v>0.01852821163101581</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1809983626337829</v>
+        <v>0.007233415853902248</v>
       </c>
       <c r="N2" t="n">
-        <v>0.05389140889910647</v>
+        <v>0.001508589736131454</v>
       </c>
       <c r="O2" t="n">
-        <v>0.01139631716997219</v>
+        <v>0.0001923620194541665</v>
       </c>
       <c r="P2" t="n">
-        <v>0.004456152191424411</v>
+        <v>0.002347137404440196</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0003105898036025931</v>
+        <v>0.0003112148743858184</v>
       </c>
       <c r="R2" t="n">
-        <v>9.018745742986297e-05</v>
+        <v>7.220865600481225e-06</v>
       </c>
       <c r="S2" t="n">
-        <v>8.853540205706458e-06</v>
+        <v>6.954849359679569e-07</v>
       </c>
       <c r="T2" t="n">
-        <v>6.998312156167471e-07</v>
+        <v>1.843817546047509e-06</v>
       </c>
       <c r="U2" t="n">
-        <v>4.430037478310536e-08</v>
+        <v>1.339282884471993e-07</v>
       </c>
       <c r="V2" t="n">
-        <v>3.330251634544979e-09</v>
+        <v>1.653003860255796e-08</v>
       </c>
       <c r="W2" t="n">
-        <v>2.085399387101214e-10</v>
+        <v>3.415665984901628e-10</v>
       </c>
       <c r="X2" t="n">
-        <v>1.005908770940212e-11</v>
+        <v>4.102614019315197e-11</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.738735198803591e-13</v>
+        <v>1.824193059206669e-12</v>
       </c>
       <c r="Z2" t="n">
-        <v>4.007613245680327e-15</v>
+        <v>8.288012514336875e-14</v>
       </c>
       <c r="AA2" t="n">
-        <v>4.691475187528812e-16</v>
+        <v>6.919387580354379e-15</v>
       </c>
       <c r="AB2" t="n">
-        <v>3.17952118379181e-17</v>
+        <v>3.293660536688149e-16</v>
       </c>
       <c r="AC2" t="n">
-        <v>6.32930761244944e-19</v>
+        <v>1.629030608761627e-17</v>
       </c>
       <c r="AD2" t="n">
-        <v>5.153967384920564e-21</v>
+        <v>1.463469413388891e-19</v>
       </c>
       <c r="AE2" t="n">
-        <v>2.290644688764778e-22</v>
+        <v>7.887441771983019e-21</v>
       </c>
       <c r="AF2" t="n">
-        <v>9.06422458033888e-25</v>
+        <v>6.838958138852547e-21</v>
       </c>
       <c r="AG2" t="n">
-        <v>8.65661444039492e-27</v>
+        <v>9.506152316096339e-22</v>
       </c>
       <c r="AH2" t="n">
-        <v>7.738775188606195e-29</v>
+        <v>5.702700317549954e-23</v>
       </c>
       <c r="AI2" t="n">
-        <v>1.067109164075261e-30</v>
+        <v>1.293655669964994e-24</v>
       </c>
       <c r="AJ2" t="n">
-        <v>6.297562225714605e-33</v>
+        <v>7.633834412276685e-27</v>
       </c>
       <c r="AK2" t="n">
-        <v>1.799626856990218e-35</v>
+        <v>8.738076261986586e-29</v>
       </c>
       <c r="AL2" t="n">
-        <v>1.086138112160119e-37</v>
+        <v>4.371773000327412e-30</v>
       </c>
       <c r="AM2" t="n">
-        <v>4.214014965827184e-40</v>
+        <v>9.398990492720426e-32</v>
       </c>
       <c r="AN2" t="n">
-        <v>7.847510480832911e-43</v>
+        <v>4.653726140169607e-33</v>
       </c>
       <c r="AO2" t="n">
-        <v>5.549957260831971e-44</v>
+        <v>6.01789883138508e-35</v>
       </c>
       <c r="AP2" t="n">
-        <v>7.373560076580769e-47</v>
+        <v>2.908395070810757e-36</v>
       </c>
       <c r="AQ2" t="n">
-        <v>8.67497357805241e-49</v>
+        <v>2.125966894560218e-37</v>
       </c>
       <c r="AR2" t="n">
-        <v>1.963351768337856e-51</v>
+        <v>9.913580614910273e-36</v>
       </c>
       <c r="AS2" t="n">
-        <v>7.049529833398059e-54</v>
+        <v>4.216097044954992e-37</v>
       </c>
       <c r="AT2" t="n">
-        <v>1.599145090471458e-56</v>
+        <v>2.344608810459595e-38</v>
       </c>
       <c r="AU2" t="n">
-        <v>8.037915593052252e-59</v>
+        <v>5.8620594858079e-40</v>
       </c>
       <c r="AV2" t="n">
-        <v>1.069662042388981e-60</v>
+        <v>7.258626552208991e-42</v>
       </c>
       <c r="AW2" t="n">
-        <v>2.008255337802556e-63</v>
+        <v>1.656798321931057e-43</v>
       </c>
       <c r="AX2" t="n">
-        <v>1.415044566799757e-65</v>
+        <v>9.089526065687036e-46</v>
       </c>
       <c r="AY2" t="n">
-        <v>4.110192440018294e-68</v>
+        <v>1.94133215285932e-47</v>
       </c>
       <c r="AZ2" t="n">
-        <v>5.479423986024091e-71</v>
+        <v>3.957001883126482e-49</v>
       </c>
       <c r="BA2" t="n">
-        <v>3.347466810256009e-74</v>
+        <v>3.179417978749659e-51</v>
       </c>
       <c r="BB2" t="n">
-        <v>3.673237698994905e-77</v>
+        <v>4.012037846702313e-52</v>
       </c>
       <c r="BC2" t="n">
-        <v>4.404685443848926e-80</v>
+        <v>4.785634893543239e-54</v>
       </c>
       <c r="BD2" t="n">
-        <v>2.000301869146922e-83</v>
+        <v>2.45068930719465e-55</v>
       </c>
       <c r="BE2" t="n">
-        <v>7.111573449343491e-86</v>
+        <v>5.952145135274508e-57</v>
       </c>
       <c r="BF2" t="n">
-        <v>1.603214980663906e-88</v>
+        <v>3.711903981381361e-59</v>
       </c>
       <c r="BG2" t="n">
-        <v>3.696298781549676e-91</v>
+        <v>7.358583774060491e-61</v>
       </c>
       <c r="BH2" t="n">
-        <v>2.626263547141e-94</v>
+        <v>1.352209421814595e-62</v>
       </c>
       <c r="BI2" t="n">
-        <v>1.26412794471349e-96</v>
+        <v>1.586013753514117e-64</v>
       </c>
       <c r="BJ2" t="n">
-        <v>2.607690102810432e-99</v>
+        <v>1.747343784115512e-66</v>
       </c>
       <c r="BK2" t="n">
-        <v>2.610701116092577e-102</v>
+        <v>1.906143594454978e-68</v>
       </c>
       <c r="BL2" t="n">
-        <v>2.504230277283315e-105</v>
+        <v>1.532673682914242e-69</v>
       </c>
       <c r="BM2" t="n">
-        <v>1.228479308903223e-108</v>
+        <v>1.90131847799743e-71</v>
       </c>
       <c r="BN2" t="n">
-        <v>1.027523281265541e-111</v>
+        <v>8.440596627139645e-74</v>
       </c>
       <c r="BO2" t="n">
-        <v>6.746293622149245e-115</v>
+        <v>1.105025479798426e-75</v>
       </c>
       <c r="BP2" t="n">
-        <v>1.058833676994947e-117</v>
+        <v>9.979693879304559e-78</v>
       </c>
       <c r="BQ2" t="n">
-        <v>7.024173522708374e-121</v>
+        <v>1.55804611774116e-79</v>
       </c>
       <c r="BR2" t="n">
-        <v>7.762743333905189e-124</v>
+        <v>1.156469553904717e-81</v>
       </c>
       <c r="BS2" t="n">
-        <v>6.406037632369312e-127</v>
+        <v>7.31329416683587e-83</v>
       </c>
       <c r="BT2" t="n">
-        <v>6.485829358889627e-130</v>
+        <v>5.226211278842586e-85</v>
       </c>
       <c r="BU2" t="n">
-        <v>6.679917041893379e-133</v>
+        <v>9.673081873229019e-87</v>
       </c>
       <c r="BV2" t="n">
-        <v>3.088236862994553e-136</v>
+        <v>7.97769124113343e-89</v>
       </c>
       <c r="BW2" t="n">
-        <v>1.093801270385732e-139</v>
+        <v>2.693441458133223e-90</v>
       </c>
       <c r="BX2" t="n">
-        <v>1.196566320568147e-142</v>
+        <v>1.609873876657949e-92</v>
       </c>
       <c r="BY2" t="n">
-        <v>1.138809822115616e-145</v>
+        <v>2.169099533229228e-94</v>
       </c>
       <c r="BZ2" t="n">
-        <v>8.395611362303432e-149</v>
+        <v>8.264651124905639e-96</v>
       </c>
       <c r="CA2" t="n">
-        <v>4.17450228625175e-152</v>
+        <v>9.834420989363401e-98</v>
       </c>
       <c r="CB2" t="n">
-        <v>2.341017671130138e-155</v>
+        <v>8.85665834881697e-100</v>
       </c>
       <c r="CC2" t="n">
-        <v>1.037596513689565e-158</v>
+        <v>1.412429531205957e-101</v>
       </c>
       <c r="CD2" t="n">
-        <v>3.377609757156424e-162</v>
+        <v>1.046138015787134e-103</v>
       </c>
       <c r="CE2" t="n">
-        <v>8.761517123355903e-166</v>
+        <v>1.321446428318846e-105</v>
       </c>
       <c r="CF2" t="n">
-        <v>3.674386170749284e-169</v>
+        <v>2.929928456681318e-107</v>
       </c>
       <c r="CG2" t="n">
-        <v>1.743446920328931e-172</v>
+        <v>3.897222009701415e-109</v>
       </c>
       <c r="CH2" t="n">
-        <v>7.133230665809399e-176</v>
+        <v>3.31584612324026e-111</v>
       </c>
       <c r="CI2" t="n">
-        <v>2.493433797766092e-179</v>
+        <v>3.345347672276913e-113</v>
       </c>
       <c r="CJ2" t="n">
-        <v>2.638050247293165e-182</v>
+        <v>1.131921434977828e-114</v>
       </c>
       <c r="CK2" t="n">
-        <v>9.24533411041465e-186</v>
+        <v>8.530847032486287e-117</v>
       </c>
       <c r="CL2" t="n">
-        <v>2.192625096671855e-189</v>
+        <v>5.269526395623134e-119</v>
       </c>
       <c r="CM2" t="n">
-        <v>8.526476248350999e-193</v>
+        <v>6.929083489205595e-121</v>
       </c>
       <c r="CN2" t="n">
-        <v>3.965227744706711e-196</v>
+        <v>9.169644737293053e-123</v>
       </c>
       <c r="CO2" t="n">
-        <v>1.330677357904262e-199</v>
+        <v>1.106632952822203e-124</v>
       </c>
       <c r="CP2" t="n">
-        <v>2.237023907828217e-203</v>
+        <v>3.742355681446546e-126</v>
       </c>
       <c r="CQ2" t="n">
-        <v>1.131916439971754e-206</v>
+        <v>1.4158972768932e-127</v>
       </c>
       <c r="CR2" t="n">
-        <v>2.134616866058326e-210</v>
+        <v>3.894009117483287e-129</v>
       </c>
       <c r="CS2" t="n">
-        <v>7.407232268700287e-214</v>
+        <v>2.284572060004385e-131</v>
       </c>
       <c r="CT2" t="n">
-        <v>2.634191410751378e-217</v>
+        <v>2.18020215718934e-133</v>
       </c>
       <c r="CU2" t="n">
-        <v>4.975804205362544e-221</v>
+        <v>2.346642974945549e-135</v>
       </c>
       <c r="CV2" t="n">
-        <v>2.01939398664095e-224</v>
+        <v>1.295696439767341e-137</v>
       </c>
       <c r="CW2" t="n">
-        <v>7.427586281507632e-228</v>
+        <v>1.036752897174498e-139</v>
       </c>
       <c r="CX2" t="n">
-        <v>3.332186332196852e-231</v>
+        <v>2.09877898811366e-141</v>
       </c>
       <c r="CY2" t="n">
-        <v>1.255138472959461e-234</v>
+        <v>1.333903423238693e-143</v>
       </c>
       <c r="CZ2" t="n">
-        <v>3.747562280970759e-238</v>
+        <v>7.191896194642446e-146</v>
       </c>
       <c r="DA2" t="n">
-        <v>1.103193155417665e-241</v>
+        <v>4.145524294584282e-148</v>
       </c>
       <c r="DB2" t="n">
-        <v>2.812548212095146e-245</v>
+        <v>2.8462042406981e-150</v>
       </c>
       <c r="DC2" t="n">
-        <v>6.134558115571087e-249</v>
+        <v>4.025871929100632e-152</v>
       </c>
       <c r="DD2" t="n">
-        <v>5.256484722266205e-252</v>
+        <v>2.319348386754155e-154</v>
       </c>
       <c r="DE2" t="n">
-        <v>7.36206191804088e-256</v>
+        <v>1.780668429521543e-156</v>
       </c>
       <c r="DF2" t="n">
-        <v>1.692101639056791e-259</v>
+        <v>1.361673468111219e-158</v>
       </c>
       <c r="DG2" t="n">
-        <v>2.204793702601369e-263</v>
+        <v>1.554899817880129e-159</v>
       </c>
       <c r="DH2" t="n">
-        <v>9.411371149187703e-267</v>
+        <v>1.161859867328723e-160</v>
       </c>
       <c r="DI2" t="n">
-        <v>5.057701710626856e-270</v>
+        <v>2.261996249191347e-162</v>
       </c>
       <c r="DJ2" t="n">
-        <v>1.59887997653854e-273</v>
+        <v>1.4842536927861e-164</v>
       </c>
       <c r="DK2" t="n">
-        <v>3.319471428691836e-277</v>
+        <v>7.602511668885596e-167</v>
       </c>
       <c r="DL2" t="n">
-        <v>6.257899117532706e-281</v>
+        <v>1.604893925242449e-168</v>
       </c>
       <c r="DM2" t="n">
-        <v>5.815479050537436e-285</v>
+        <v>1.272470368446676e-170</v>
       </c>
       <c r="DN2" t="n">
-        <v>3.057509728698062e-288</v>
+        <v>7.02271460628645e-173</v>
       </c>
       <c r="DO2" t="n">
-        <v>8.678965913802229e-292</v>
+        <v>5.573752364119072e-175</v>
       </c>
       <c r="DP2" t="n">
-        <v>3.089903519477134e-295</v>
+        <v>1.33251867099914e-176</v>
       </c>
       <c r="DQ2" t="n">
-        <v>7.879275523640203e-299</v>
+        <v>2.186451735241108e-178</v>
       </c>
       <c r="DR2" t="n">
-        <v>1.554567312501098e-302</v>
+        <v>1.09301045649813e-180</v>
       </c>
       <c r="DS2" t="n">
-        <v>2.407276866846188e-306</v>
+        <v>1.944564189040506e-182</v>
       </c>
       <c r="DT2" t="n">
-        <v>0</v>
+        <v>1.9135367377323e-184</v>
       </c>
       <c r="DU2" t="n">
-        <v>0</v>
+        <v>2.999587212242996e-186</v>
       </c>
       <c r="DV2" t="n">
-        <v>0</v>
+        <v>1.949162363982139e-188</v>
       </c>
       <c r="DW2" t="n">
-        <v>0</v>
+        <v>1.670326586666645e-190</v>
       </c>
       <c r="DX2" t="n">
-        <v>0</v>
+        <v>7.935705375203635e-193</v>
       </c>
       <c r="DY2" t="n">
-        <v>0</v>
+        <v>7.701494125639579e-195</v>
       </c>
       <c r="DZ2" t="n">
-        <v>0</v>
+        <v>6.67440061294836e-197</v>
       </c>
       <c r="EA2" t="n">
-        <v>0</v>
+        <v>2.874731544839126e-199</v>
       </c>
       <c r="EB2" t="n">
-        <v>0</v>
+        <v>1.801990206441032e-201</v>
       </c>
       <c r="EC2" t="n">
-        <v>0</v>
+        <v>2.459642354678996e-203</v>
       </c>
       <c r="ED2" t="n">
-        <v>0</v>
+        <v>1.135738669014035e-205</v>
       </c>
       <c r="EE2" t="n">
-        <v>0</v>
+        <v>1.663563595487488e-207</v>
       </c>
       <c r="EF2" t="n">
-        <v>0</v>
+        <v>5.666251510462112e-209</v>
       </c>
       <c r="EG2" t="n">
-        <v>0</v>
+        <v>3.311245585567583e-211</v>
       </c>
       <c r="EH2" t="n">
-        <v>0</v>
+        <v>5.302493683371268e-213</v>
       </c>
       <c r="EI2" t="n">
-        <v>0</v>
+        <v>6.028267799010024e-215</v>
       </c>
       <c r="EJ2" t="n">
-        <v>0</v>
+        <v>5.448948748932872e-217</v>
       </c>
       <c r="EK2" t="n">
-        <v>0</v>
+        <v>2.229651699475948e-219</v>
       </c>
       <c r="EL2" t="n">
-        <v>0</v>
+        <v>9.869365906194322e-222</v>
       </c>
       <c r="EM2" t="n">
-        <v>0</v>
+        <v>1.075906456451805e-223</v>
       </c>
       <c r="EN2" t="n">
-        <v>0</v>
+        <v>4.530208883596322e-226</v>
       </c>
       <c r="EO2" t="n">
-        <v>0</v>
+        <v>2.065725062476087e-228</v>
       </c>
       <c r="EP2" t="n">
-        <v>0</v>
+        <v>1.44668117669185e-230</v>
       </c>
       <c r="EQ2" t="n">
-        <v>0</v>
+        <v>7.315679072260333e-233</v>
       </c>
       <c r="ER2" t="n">
-        <v>0</v>
+        <v>4.063055185341211e-235</v>
       </c>
       <c r="ES2" t="n">
-        <v>0</v>
+        <v>5.00808118741808e-237</v>
       </c>
       <c r="ET2" t="n">
-        <v>0</v>
+        <v>2.008674942784371e-239</v>
       </c>
       <c r="EU2" t="n">
-        <v>0</v>
+        <v>2.002337636750125e-241</v>
       </c>
       <c r="EV2" t="n">
-        <v>0</v>
+        <v>2.119737385787236e-243</v>
       </c>
       <c r="EW2" t="n">
-        <v>0</v>
+        <v>1.11700750904613e-245</v>
       </c>
       <c r="EX2" t="n">
-        <v>0</v>
+        <v>7.256576636907232e-248</v>
       </c>
       <c r="EY2" t="n">
-        <v>0</v>
+        <v>4.257043740245907e-250</v>
       </c>
       <c r="EZ2" t="n">
-        <v>0</v>
+        <v>2.101898708331e-252</v>
       </c>
       <c r="FA2" t="n">
-        <v>0</v>
+        <v>1.4369767023244e-254</v>
       </c>
       <c r="FB2" t="n">
-        <v>0</v>
+        <v>3.404672427439888e-256</v>
       </c>
       <c r="FC2" t="n">
-        <v>0</v>
+        <v>3.996450463891071e-258</v>
       </c>
       <c r="FD2" t="n">
-        <v>0</v>
+        <v>2.040273003527644e-260</v>
       </c>
       <c r="FE2" t="n">
-        <v>0</v>
+        <v>2.690623947935355e-262</v>
       </c>
       <c r="FF2" t="n">
-        <v>0</v>
+        <v>2.908910492305739e-264</v>
       </c>
       <c r="FG2" t="n">
-        <v>0</v>
+        <v>1.691605415639637e-266</v>
       </c>
       <c r="FH2" t="n">
-        <v>0</v>
+        <v>7.838005540974576e-269</v>
       </c>
       <c r="FI2" t="n">
-        <v>0</v>
+        <v>1.217496543302898e-270</v>
       </c>
       <c r="FJ2" t="n">
-        <v>0</v>
+        <v>1.730333945835313e-272</v>
       </c>
       <c r="FK2" t="n">
-        <v>0</v>
+        <v>3.733947463793277e-274</v>
       </c>
       <c r="FL2" t="n">
-        <v>0</v>
+        <v>1.852260756808473e-276</v>
       </c>
       <c r="FM2" t="n">
-        <v>0</v>
+        <v>7.015249440049556e-279</v>
       </c>
       <c r="FN2" t="n">
-        <v>0</v>
+        <v>6.713984216629418e-281</v>
       </c>
       <c r="FO2" t="n">
-        <v>0</v>
+        <v>2.301026464166492e-283</v>
       </c>
       <c r="FP2" t="n">
-        <v>0</v>
+        <v>7.757087768547798e-286</v>
       </c>
       <c r="FQ2" t="n">
-        <v>0</v>
+        <v>4.020127190603823e-288</v>
       </c>
       <c r="FR2" t="n">
-        <v>0</v>
+        <v>1.035895522320164e-289</v>
       </c>
       <c r="FS2" t="n">
-        <v>0</v>
+        <v>4.036562132984862e-292</v>
       </c>
       <c r="FT2" t="n">
-        <v>0</v>
+        <v>1.509839425485103e-294</v>
       </c>
       <c r="FU2" t="n">
-        <v>0</v>
+        <v>5.23273717915006e-297</v>
       </c>
       <c r="FV2" t="n">
-        <v>0</v>
+        <v>2.530006372508145e-299</v>
       </c>
       <c r="FW2" t="n">
-        <v>0</v>
+        <v>8.382701669694474e-302</v>
       </c>
       <c r="FX2" t="n">
-        <v>0</v>
+        <v>5.700690729763008e-304</v>
       </c>
       <c r="FY2" t="n">
-        <v>0</v>
+        <v>2.069976444063208e-306</v>
       </c>
       <c r="FZ2" t="n">
-        <v>0</v>
+        <v>7.26625666575755e-309</v>
       </c>
       <c r="GA2" t="n">
         <v>0</v>
@@ -9493,85 +9493,85 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3342438185630351</v>
+        <v>0.3424504765450566</v>
       </c>
       <c r="C3" t="n">
-        <v>0.335419976604495</v>
+        <v>0.3209485256857082</v>
       </c>
       <c r="D3" t="n">
-        <v>0.335419976604495</v>
+        <v>0.3209485256857082</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3366619276003915</v>
+        <v>0.3239399378356603</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3494393323379861</v>
+        <v>0.3515850652969598</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3492677306930375</v>
+        <v>0.3069851545937397</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3987867675188323</v>
+        <v>0.5486993003452287</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4494652148678985</v>
+        <v>0.6194237136816705</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4900174350863224</v>
+        <v>0.4423626979378065</v>
       </c>
       <c r="K3" t="n">
-        <v>0.6948414697967122</v>
+        <v>0.6640205782585946</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8078775576863731</v>
+        <v>0.9346004098106926</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8110944838810231</v>
+        <v>0.9028519606850999</v>
       </c>
       <c r="N3" t="n">
-        <v>0.94194684382556</v>
+        <v>0.9896084659052855</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9868622781032976</v>
+        <v>0.9981740760329774</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9953490481092064</v>
+        <v>0.9971470858179832</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9995938556441925</v>
+        <v>0.9981734343395394</v>
       </c>
       <c r="R3" t="n">
-        <v>0.99990323081468</v>
+        <v>0.9996863070600238</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9999803579226154</v>
+        <v>0.9999570037587515</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9999977631129091</v>
+        <v>0.9999879814031442</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9999997945276288</v>
+        <v>0.9999993460339804</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9999999841607302</v>
+        <v>0.9999999803310899</v>
       </c>
       <c r="W3" t="n">
-        <v>0.9999999992788481</v>
+        <v>0.9999999994493092</v>
       </c>
       <c r="X3" t="n">
-        <v>0.9999999999631192</v>
+        <v>0.9999999999530012</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.9999999999982722</v>
+        <v>0.9999999999980163</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.9999999999999426</v>
+        <v>0.9999999999998935</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.9999999999999984</v>
+        <v>0.9999999999999929</v>
       </c>
       <c r="AB3" t="n">
-        <v>1</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="AC3" t="n">
         <v>1</v>
@@ -11000,562 +11000,562 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3315129827925535</v>
+        <v>0.315105458211722</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3291614702975998</v>
+        <v>0.358094785867129</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3291614702975998</v>
+        <v>0.358094785867129</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2957417425714632</v>
+        <v>0.44500534130847</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3068223069051266</v>
+        <v>0.346314132129176</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2096414037214075</v>
+        <v>0.6202034134404942</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2091057070837963</v>
+        <v>0.3547156577121614</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1301173715103817</v>
+        <v>0.3578273793355169</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06135459380873512</v>
+        <v>0.5510986358190718</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1047805483672264</v>
+        <v>0.2905093047952551</v>
       </c>
       <c r="L4" t="n">
-        <v>0.03950961620467385</v>
+        <v>0.04687137855829154</v>
       </c>
       <c r="M4" t="n">
-        <v>0.007907153485193942</v>
+        <v>0.08991462346099789</v>
       </c>
       <c r="N4" t="n">
-        <v>0.004161747275333418</v>
+        <v>0.00888294435858299</v>
       </c>
       <c r="O4" t="n">
-        <v>0.001741404726730175</v>
+        <v>0.001633561947568583</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0001947996993690678</v>
+        <v>0.0005057767775765266</v>
       </c>
       <c r="Q4" t="n">
-        <v>9.555455220485447e-05</v>
+        <v>0.001515350786074811</v>
       </c>
       <c r="R4" t="n">
-        <v>6.581727890181774e-06</v>
+        <v>0.0003064720743757754</v>
       </c>
       <c r="S4" t="n">
-        <v>1.078853717892774e-05</v>
+        <v>4.230075631241888e-05</v>
       </c>
       <c r="T4" t="n">
-        <v>1.537055875219689e-06</v>
+        <v>1.01747793098219e-05</v>
       </c>
       <c r="U4" t="n">
-        <v>1.61171996480796e-07</v>
+        <v>5.200377311470183e-07</v>
       </c>
       <c r="V4" t="n">
-        <v>1.250901812042215e-08</v>
+        <v>3.138871432679878e-09</v>
       </c>
       <c r="W4" t="n">
-        <v>5.126119427781488e-10</v>
+        <v>2.091241568353365e-10</v>
       </c>
       <c r="X4" t="n">
-        <v>2.682176490074388e-11</v>
+        <v>5.972646925831386e-12</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.553939522327042e-12</v>
+        <v>1.594834666412038e-13</v>
       </c>
       <c r="Z4" t="n">
-        <v>5.348862421354418e-14</v>
+        <v>2.355161066089341e-14</v>
       </c>
       <c r="AA4" t="n">
-        <v>9.983455415175129e-16</v>
+        <v>2.625469405400969e-16</v>
       </c>
       <c r="AB4" t="n">
-        <v>7.188474380522176e-18</v>
+        <v>1.200130936630428e-17</v>
       </c>
       <c r="AC4" t="n">
-        <v>9.496311452553967e-20</v>
+        <v>1.218863160192474e-18</v>
       </c>
       <c r="AD4" t="n">
-        <v>5.464673749650176e-21</v>
+        <v>2.307439691265418e-19</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.670358376582293e-23</v>
+        <v>1.808829527035466e-20</v>
       </c>
       <c r="AF4" t="n">
-        <v>3.529886399715829e-25</v>
+        <v>2.625654381501159e-21</v>
       </c>
       <c r="AG4" t="n">
-        <v>2.74154885233272e-27</v>
+        <v>2.848021112218708e-22</v>
       </c>
       <c r="AH4" t="n">
-        <v>2.451309951276326e-29</v>
+        <v>1.814206803184974e-23</v>
       </c>
       <c r="AI4" t="n">
-        <v>9.753119085220602e-32</v>
+        <v>4.185484073820035e-25</v>
       </c>
       <c r="AJ4" t="n">
-        <v>9.262509340687152e-34</v>
+        <v>2.469212426679074e-26</v>
       </c>
       <c r="AK4" t="n">
-        <v>1.928066563498821e-35</v>
+        <v>1.209634345409008e-27</v>
       </c>
       <c r="AL4" t="n">
-        <v>8.028834518863385e-38</v>
+        <v>8.656064300613561e-29</v>
       </c>
       <c r="AM4" t="n">
-        <v>4.596886311040511e-40</v>
+        <v>1.441357814131444e-30</v>
       </c>
       <c r="AN4" t="n">
-        <v>5.261476702558647e-42</v>
+        <v>4.283980180989363e-32</v>
       </c>
       <c r="AO4" t="n">
-        <v>2.626321189382461e-44</v>
+        <v>9.614679972057547e-34</v>
       </c>
       <c r="AP4" t="n">
-        <v>6.009408614517632e-46</v>
+        <v>4.968803727058305e-35</v>
       </c>
       <c r="AQ4" t="n">
-        <v>3.002816309447854e-48</v>
+        <v>3.307772134108939e-36</v>
       </c>
       <c r="AR4" t="n">
-        <v>1.05546132035648e-50</v>
+        <v>4.585390068904031e-33</v>
       </c>
       <c r="AS4" t="n">
-        <v>1.493267767868567e-53</v>
+        <v>1.169162570780949e-34</v>
       </c>
       <c r="AT4" t="n">
-        <v>3.980573438756102e-56</v>
+        <v>2.139472863754869e-36</v>
       </c>
       <c r="AU4" t="n">
-        <v>4.243478511932721e-58</v>
+        <v>2.778580550616184e-38</v>
       </c>
       <c r="AV4" t="n">
-        <v>4.070622313579652e-61</v>
+        <v>1.304293848750668e-39</v>
       </c>
       <c r="AW4" t="n">
-        <v>1.215992097137732e-63</v>
+        <v>2.770887833010006e-41</v>
       </c>
       <c r="AX4" t="n">
-        <v>7.193448931507253e-67</v>
+        <v>1.138775897011782e-42</v>
       </c>
       <c r="AY4" t="n">
-        <v>5.779563630340117e-70</v>
+        <v>4.054178871843151e-44</v>
       </c>
       <c r="AZ4" t="n">
-        <v>1.198252209056888e-72</v>
+        <v>1.336978977139692e-45</v>
       </c>
       <c r="BA4" t="n">
-        <v>3.83503935989508e-75</v>
+        <v>3.485576929876918e-47</v>
       </c>
       <c r="BB4" t="n">
-        <v>1.083798165448326e-77</v>
+        <v>8.541246974267175e-48</v>
       </c>
       <c r="BC4" t="n">
-        <v>3.364084045080411e-80</v>
+        <v>7.711717213532423e-49</v>
       </c>
       <c r="BD4" t="n">
-        <v>7.400724535733639e-83</v>
+        <v>4.504681717796807e-50</v>
       </c>
       <c r="BE4" t="n">
-        <v>2.833398193211881e-86</v>
+        <v>1.311421560343835e-51</v>
       </c>
       <c r="BF4" t="n">
-        <v>2.640588880277456e-89</v>
+        <v>4.462363483224654e-53</v>
       </c>
       <c r="BG4" t="n">
-        <v>2.972965326350253e-92</v>
+        <v>7.862180923420511e-55</v>
       </c>
       <c r="BH4" t="n">
-        <v>9.937907196795185e-95</v>
+        <v>6.079648829231348e-57</v>
       </c>
       <c r="BI4" t="n">
-        <v>2.203713897148499e-96</v>
+        <v>5.914495100070257e-59</v>
       </c>
       <c r="BJ4" t="n">
-        <v>1.431265764029467e-99</v>
+        <v>8.157253063516689e-61</v>
       </c>
       <c r="BK4" t="n">
-        <v>1.136475805546567e-102</v>
+        <v>8.121773701443685e-63</v>
       </c>
       <c r="BL4" t="n">
-        <v>5.938476698051717e-106</v>
+        <v>7.969879127397193e-64</v>
       </c>
       <c r="BM4" t="n">
-        <v>4.818244676730671e-109</v>
+        <v>1.413668898297115e-65</v>
       </c>
       <c r="BN4" t="n">
-        <v>2.084215546871847e-112</v>
+        <v>5.651532500931341e-67</v>
       </c>
       <c r="BO4" t="n">
-        <v>1.137296390577057e-115</v>
+        <v>5.0202700555611e-69</v>
       </c>
       <c r="BP4" t="n">
-        <v>2.041493669467215e-119</v>
+        <v>1.071242495800362e-70</v>
       </c>
       <c r="BQ4" t="n">
-        <v>1.153570540518694e-122</v>
+        <v>7.707993256468157e-73</v>
       </c>
       <c r="BR4" t="n">
-        <v>5.63074158128298e-126</v>
+        <v>9.602378401740933e-75</v>
       </c>
       <c r="BS4" t="n">
-        <v>1.62921437405776e-129</v>
+        <v>4.58603659990179e-76</v>
       </c>
       <c r="BT4" t="n">
-        <v>3.564058977539196e-133</v>
+        <v>5.600323902796381e-78</v>
       </c>
       <c r="BU4" t="n">
-        <v>8.101074998401086e-137</v>
+        <v>1.14460116990246e-79</v>
       </c>
       <c r="BV4" t="n">
-        <v>4.519808036705295e-140</v>
+        <v>1.01523037748156e-81</v>
       </c>
       <c r="BW4" t="n">
-        <v>2.558748162899811e-143</v>
+        <v>3.24633878459084e-83</v>
       </c>
       <c r="BX4" t="n">
-        <v>9.259570689468128e-147</v>
+        <v>7.085305695100213e-85</v>
       </c>
       <c r="BY4" t="n">
-        <v>1.65322079626519e-150</v>
+        <v>4.702755247283769e-87</v>
       </c>
       <c r="BZ4" t="n">
-        <v>8.214962566741382e-154</v>
+        <v>1.19227922779164e-88</v>
       </c>
       <c r="CA4" t="n">
-        <v>2.425536676087839e-157</v>
+        <v>2.059799937037496e-90</v>
       </c>
       <c r="CB4" t="n">
-        <v>1.247550925072966e-160</v>
+        <v>2.759398953376549e-92</v>
       </c>
       <c r="CC4" t="n">
-        <v>3.726467070897732e-164</v>
+        <v>3.436850486399208e-94</v>
       </c>
       <c r="CD4" t="n">
-        <v>1.096020259373586e-166</v>
+        <v>4.131271767916929e-96</v>
       </c>
       <c r="CE4" t="n">
-        <v>4.976623614957553e-170</v>
+        <v>8.761928937888436e-98</v>
       </c>
       <c r="CF4" t="n">
-        <v>1.347080125286817e-173</v>
+        <v>1.862721236759321e-99</v>
       </c>
       <c r="CG4" t="n">
-        <v>2.991761109514152e-177</v>
+        <v>4.862664739950733e-101</v>
       </c>
       <c r="CH4" t="n">
-        <v>9.037555098733869e-181</v>
+        <v>6.055848817018728e-103</v>
       </c>
       <c r="CI4" t="n">
-        <v>4.72475304461973e-184</v>
+        <v>3.91647539324287e-105</v>
       </c>
       <c r="CJ4" t="n">
-        <v>2.302665917012035e-187</v>
+        <v>2.382863976386076e-106</v>
       </c>
       <c r="CK4" t="n">
-        <v>5.845942943203758e-191</v>
+        <v>1.777113267018072e-108</v>
       </c>
       <c r="CL4" t="n">
-        <v>2.20660999064334e-194</v>
+        <v>2.505603766384307e-110</v>
       </c>
       <c r="CM4" t="n">
-        <v>8.856117505665877e-198</v>
+        <v>5.127619763911967e-112</v>
       </c>
       <c r="CN4" t="n">
-        <v>2.414606364045393e-201</v>
+        <v>5.802719026243778e-114</v>
       </c>
       <c r="CO4" t="n">
-        <v>7.886479064794744e-205</v>
+        <v>7.86883138658294e-116</v>
       </c>
       <c r="CP4" t="n">
-        <v>3.637950372234623e-208</v>
+        <v>4.434897355579763e-117</v>
       </c>
       <c r="CQ4" t="n">
-        <v>5.491023436921603e-212</v>
+        <v>9.441492120798438e-119</v>
       </c>
       <c r="CR4" t="n">
-        <v>2.565363481165838e-215</v>
+        <v>3.108504127855064e-120</v>
       </c>
       <c r="CS4" t="n">
-        <v>5.672702739214169e-219</v>
+        <v>4.347663709197128e-122</v>
       </c>
       <c r="CT4" t="n">
-        <v>1.847010224754285e-222</v>
+        <v>3.018781617761277e-124</v>
       </c>
       <c r="CU4" t="n">
-        <v>9.736563832697996e-226</v>
+        <v>4.995276619069485e-126</v>
       </c>
       <c r="CV4" t="n">
-        <v>3.275383021291393e-229</v>
+        <v>3.487481044345105e-128</v>
       </c>
       <c r="CW4" t="n">
-        <v>4.894295116611807e-233</v>
+        <v>4.591893820730073e-130</v>
       </c>
       <c r="CX4" t="n">
-        <v>6.975049846062387e-237</v>
+        <v>1.322051062340819e-131</v>
       </c>
       <c r="CY4" t="n">
-        <v>2.792732647502641e-240</v>
+        <v>2.153742963065414e-133</v>
       </c>
       <c r="CZ4" t="n">
-        <v>9.675351594593454e-244</v>
+        <v>1.61656792492798e-135</v>
       </c>
       <c r="DA4" t="n">
-        <v>1.781493542641172e-247</v>
+        <v>8.931453706118732e-138</v>
       </c>
       <c r="DB4" t="n">
-        <v>3.696808818093951e-251</v>
+        <v>4.863283084501453e-140</v>
       </c>
       <c r="DC4" t="n">
-        <v>8.26565777232127e-255</v>
+        <v>1.274040888385202e-141</v>
       </c>
       <c r="DD4" t="n">
-        <v>3.862090697421696e-258</v>
+        <v>7.710347038852775e-144</v>
       </c>
       <c r="DE4" t="n">
-        <v>1.111210342242622e-261</v>
+        <v>6.934971898056461e-146</v>
       </c>
       <c r="DF4" t="n">
-        <v>1.969441050032561e-265</v>
+        <v>4.738150782603593e-148</v>
       </c>
       <c r="DG4" t="n">
-        <v>7.431683390036396e-269</v>
+        <v>8.47803797312886e-149</v>
       </c>
       <c r="DH4" t="n">
-        <v>5.949984939420831e-272</v>
+        <v>4.112724923506563e-150</v>
       </c>
       <c r="DI4" t="n">
-        <v>2.625793591599215e-275</v>
+        <v>2.128586988190093e-152</v>
       </c>
       <c r="DJ4" t="n">
-        <v>4.219795359029039e-279</v>
+        <v>1.106543335288285e-154</v>
       </c>
       <c r="DK4" t="n">
-        <v>9.560483219089981e-283</v>
+        <v>8.206762463110954e-157</v>
       </c>
       <c r="DL4" t="n">
-        <v>4.550368337306462e-286</v>
+        <v>1.25862554418953e-158</v>
       </c>
       <c r="DM4" t="n">
-        <v>1.524190147681011e-289</v>
+        <v>1.463971804046675e-160</v>
       </c>
       <c r="DN4" t="n">
-        <v>1.873915732334653e-293</v>
+        <v>6.954035468707869e-163</v>
       </c>
       <c r="DO4" t="n">
-        <v>7.107009713766527e-297</v>
+        <v>5.85501662427764e-165</v>
       </c>
       <c r="DP4" t="n">
-        <v>7.77596766589043e-301</v>
+        <v>1.765551633567309e-166</v>
       </c>
       <c r="DQ4" t="n">
-        <v>9.576728262462381e-305</v>
+        <v>2.654660550316915e-168</v>
       </c>
       <c r="DR4" t="n">
-        <v>0</v>
+        <v>1.415126409455841e-170</v>
       </c>
       <c r="DS4" t="n">
-        <v>0</v>
+        <v>2.312042670450667e-172</v>
       </c>
       <c r="DT4" t="n">
-        <v>0</v>
+        <v>2.327636740737594e-174</v>
       </c>
       <c r="DU4" t="n">
-        <v>0</v>
+        <v>1.951285843162375e-176</v>
       </c>
       <c r="DV4" t="n">
-        <v>0</v>
+        <v>8.833325321375751e-179</v>
       </c>
       <c r="DW4" t="n">
-        <v>0</v>
+        <v>1.146573652573543e-180</v>
       </c>
       <c r="DX4" t="n">
-        <v>0</v>
+        <v>6.20497441779672e-183</v>
       </c>
       <c r="DY4" t="n">
-        <v>0</v>
+        <v>6.932867282833964e-185</v>
       </c>
       <c r="DZ4" t="n">
-        <v>0</v>
+        <v>3.704696988687365e-187</v>
       </c>
       <c r="EA4" t="n">
-        <v>0</v>
+        <v>2.075897137318827e-189</v>
       </c>
       <c r="EB4" t="n">
-        <v>0</v>
+        <v>1.269847323673714e-191</v>
       </c>
       <c r="EC4" t="n">
-        <v>0</v>
+        <v>1.880600109099822e-193</v>
       </c>
       <c r="ED4" t="n">
-        <v>0</v>
+        <v>8.624357697192503e-196</v>
       </c>
       <c r="EE4" t="n">
-        <v>0</v>
+        <v>2.111830564489277e-197</v>
       </c>
       <c r="EF4" t="n">
-        <v>0</v>
+        <v>8.004770619313857e-199</v>
       </c>
       <c r="EG4" t="n">
-        <v>0</v>
+        <v>6.032837938140418e-201</v>
       </c>
       <c r="EH4" t="n">
-        <v>0</v>
+        <v>6.248140533298838e-203</v>
       </c>
       <c r="EI4" t="n">
-        <v>0</v>
+        <v>4.801128782022437e-205</v>
       </c>
       <c r="EJ4" t="n">
-        <v>0</v>
+        <v>4.663116876377755e-207</v>
       </c>
       <c r="EK4" t="n">
-        <v>0</v>
+        <v>2.17368560983209e-209</v>
       </c>
       <c r="EL4" t="n">
-        <v>0</v>
+        <v>9.06525400324407e-212</v>
       </c>
       <c r="EM4" t="n">
-        <v>0</v>
+        <v>9.152195244270394e-214</v>
       </c>
       <c r="EN4" t="n">
-        <v>0</v>
+        <v>5.743793260168e-216</v>
       </c>
       <c r="EO4" t="n">
-        <v>0</v>
+        <v>4.785159826184715e-218</v>
       </c>
       <c r="EP4" t="n">
-        <v>0</v>
+        <v>3.808997162437931e-220</v>
       </c>
       <c r="EQ4" t="n">
-        <v>0</v>
+        <v>1.733947355462058e-222</v>
       </c>
       <c r="ER4" t="n">
-        <v>0</v>
+        <v>9.45929650004059e-225</v>
       </c>
       <c r="ES4" t="n">
-        <v>0</v>
+        <v>7.978909447254369e-227</v>
       </c>
       <c r="ET4" t="n">
-        <v>0</v>
+        <v>3.214658491528563e-229</v>
       </c>
       <c r="EU4" t="n">
-        <v>0</v>
+        <v>2.613532515832059e-231</v>
       </c>
       <c r="EV4" t="n">
-        <v>0</v>
+        <v>5.003831242586746e-233</v>
       </c>
       <c r="EW4" t="n">
-        <v>0</v>
+        <v>2.166953919978853e-235</v>
       </c>
       <c r="EX4" t="n">
-        <v>0</v>
+        <v>2.220115501684566e-237</v>
       </c>
       <c r="EY4" t="n">
-        <v>0</v>
+        <v>1.287265088994906e-239</v>
       </c>
       <c r="EZ4" t="n">
-        <v>0</v>
+        <v>1.015594659607941e-241</v>
       </c>
       <c r="FA4" t="n">
-        <v>0</v>
+        <v>1.174660333417141e-243</v>
       </c>
       <c r="FB4" t="n">
-        <v>0</v>
+        <v>3.328800765234629e-245</v>
       </c>
       <c r="FC4" t="n">
-        <v>0</v>
+        <v>3.605404507862799e-247</v>
       </c>
       <c r="FD4" t="n">
-        <v>0</v>
+        <v>2.062970519818563e-249</v>
       </c>
       <c r="FE4" t="n">
-        <v>0</v>
+        <v>3.188086098614724e-251</v>
       </c>
       <c r="FF4" t="n">
-        <v>0</v>
+        <v>1.971296509017268e-253</v>
       </c>
       <c r="FG4" t="n">
-        <v>0</v>
+        <v>9.903696650801892e-256</v>
       </c>
       <c r="FH4" t="n">
-        <v>0</v>
+        <v>9.154507698362332e-258</v>
       </c>
       <c r="FI4" t="n">
-        <v>0</v>
+        <v>1.113954669815691e-259</v>
       </c>
       <c r="FJ4" t="n">
-        <v>0</v>
+        <v>1.791942482372958e-261</v>
       </c>
       <c r="FK4" t="n">
-        <v>0</v>
+        <v>4.415729688479215e-263</v>
       </c>
       <c r="FL4" t="n">
-        <v>0</v>
+        <v>2.265166538616833e-265</v>
       </c>
       <c r="FM4" t="n">
-        <v>0</v>
+        <v>9.171820800441092e-268</v>
       </c>
       <c r="FN4" t="n">
-        <v>0</v>
+        <v>7.764912114569044e-270</v>
       </c>
       <c r="FO4" t="n">
-        <v>0</v>
+        <v>2.682438376786804e-272</v>
       </c>
       <c r="FP4" t="n">
-        <v>0</v>
+        <v>9.15726315383475e-275</v>
       </c>
       <c r="FQ4" t="n">
-        <v>0</v>
+        <v>5.732375410589719e-277</v>
       </c>
       <c r="FR4" t="n">
-        <v>0</v>
+        <v>2.932649067700185e-278</v>
       </c>
       <c r="FS4" t="n">
-        <v>0</v>
+        <v>1.691003724541111e-280</v>
       </c>
       <c r="FT4" t="n">
-        <v>0</v>
+        <v>6.223861103523804e-283</v>
       </c>
       <c r="FU4" t="n">
-        <v>0</v>
+        <v>2.153502721089302e-285</v>
       </c>
       <c r="FV4" t="n">
-        <v>0</v>
+        <v>9.160259728094423e-288</v>
       </c>
       <c r="FW4" t="n">
-        <v>0</v>
+        <v>3.575305798262743e-290</v>
       </c>
       <c r="FX4" t="n">
-        <v>0</v>
+        <v>2.929920008566875e-292</v>
       </c>
       <c r="FY4" t="n">
-        <v>0</v>
+        <v>1.592333604913822e-294</v>
       </c>
       <c r="FZ4" t="n">
-        <v>0</v>
+        <v>7.853414251157955e-297</v>
       </c>
       <c r="GA4" t="n">
-        <v>0</v>
+        <v>3.482055104604061e-299</v>
       </c>
       <c r="GB4" t="n">
-        <v>0</v>
+        <v>1.275119457782994e-301</v>
       </c>
       <c r="GC4" t="n">
-        <v>0</v>
+        <v>1.022772863628102e-303</v>
       </c>
       <c r="GD4" t="n">
-        <v>0</v>
+        <v>4.006278056075513e-306</v>
       </c>
       <c r="GE4" t="n">
-        <v>0</v>
+        <v>1.323767172038851e-308</v>
       </c>
       <c r="GF4" t="n">
         <v>0</v>
@@ -14028,385 +14028,385 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3348049366407064</v>
+        <v>0.3219045540589698</v>
       </c>
       <c r="C2" t="n">
-        <v>0.336275547543454</v>
+        <v>0.3109337859318598</v>
       </c>
       <c r="D2" t="n">
-        <v>0.336275547543454</v>
+        <v>0.3109337859318598</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3387321199613567</v>
+        <v>0.2919609440954937</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2876163075276393</v>
+        <v>0.2798964953577548</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1786024747301293</v>
+        <v>0.07617132468095826</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1218823866776671</v>
+        <v>0.01659995727157624</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1553373965702738</v>
+        <v>0.001482275947540368</v>
       </c>
       <c r="J2" t="n">
-        <v>0.10976041339175</v>
+        <v>5.08193363955692e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>0.02090444935755103</v>
+        <v>2.853466065930689e-06</v>
       </c>
       <c r="L2" t="n">
-        <v>0.01168499473352071</v>
+        <v>1.320141183187028e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0005346532780580433</v>
+        <v>2.921449504450652e-09</v>
       </c>
       <c r="N2" t="n">
-        <v>3.29831601707951e-05</v>
+        <v>7.336855632745218e-11</v>
       </c>
       <c r="O2" t="n">
-        <v>8.572459758869251e-07</v>
+        <v>1.919194043911421e-12</v>
       </c>
       <c r="P2" t="n">
-        <v>1.031243229397274e-08</v>
+        <v>9.993972467765308e-14</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.950378088881792e-10</v>
+        <v>1.469346468559291e-15</v>
       </c>
       <c r="R2" t="n">
-        <v>2.353049518234496e-12</v>
+        <v>1.603478654355463e-17</v>
       </c>
       <c r="S2" t="n">
-        <v>8.109161738311359e-15</v>
+        <v>2.776440982923495e-19</v>
       </c>
       <c r="T2" t="n">
-        <v>1.961526310991779e-16</v>
+        <v>1.173741429163348e-21</v>
       </c>
       <c r="U2" t="n">
-        <v>1.892681016875753e-18</v>
+        <v>3.603808335213059e-23</v>
       </c>
       <c r="V2" t="n">
-        <v>2.858864655432385e-21</v>
+        <v>6.889473150705972e-26</v>
       </c>
       <c r="W2" t="n">
-        <v>6.715270843497354e-24</v>
+        <v>3.734159347533758e-28</v>
       </c>
       <c r="X2" t="n">
-        <v>1.012834789182448e-26</v>
+        <v>2.28916799470049e-30</v>
       </c>
       <c r="Y2" t="n">
-        <v>9.53110076965217e-29</v>
+        <v>1.135404586752172e-32</v>
       </c>
       <c r="Z2" t="n">
-        <v>5.701459474341735e-32</v>
+        <v>1.401675526134069e-34</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.011835600206384e-35</v>
+        <v>2.513216551962805e-37</v>
       </c>
       <c r="AB2" t="n">
-        <v>7.976409189199537e-39</v>
+        <v>3.379408328611089e-39</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.689955162639793e-42</v>
+        <v>5.026892891403176e-41</v>
       </c>
       <c r="AD2" t="n">
-        <v>3.65335817773287e-46</v>
+        <v>2.034807152418632e-43</v>
       </c>
       <c r="AE2" t="n">
-        <v>5.348668786724657e-50</v>
+        <v>6.906109959984045e-46</v>
       </c>
       <c r="AF2" t="n">
-        <v>2.08576362730663e-53</v>
+        <v>8.020087428454817e-48</v>
       </c>
       <c r="AG2" t="n">
-        <v>2.246311214814894e-57</v>
+        <v>1.533859474375818e-49</v>
       </c>
       <c r="AH2" t="n">
-        <v>1.799668481582733e-60</v>
+        <v>3.949121578845012e-51</v>
       </c>
       <c r="AI2" t="n">
-        <v>3.727399443220759e-64</v>
+        <v>5.157621163854505e-53</v>
       </c>
       <c r="AJ2" t="n">
-        <v>9.042660898530862e-68</v>
+        <v>6.471142978207489e-55</v>
       </c>
       <c r="AK2" t="n">
-        <v>4.122134080061329e-71</v>
+        <v>2.291616637157948e-57</v>
       </c>
       <c r="AL2" t="n">
-        <v>2.212483623074576e-74</v>
+        <v>4.276815420017938e-60</v>
       </c>
       <c r="AM2" t="n">
-        <v>2.014202757656052e-77</v>
+        <v>5.707414842925287e-63</v>
       </c>
       <c r="AN2" t="n">
-        <v>5.791896624505577e-81</v>
+        <v>1.039006062790948e-65</v>
       </c>
       <c r="AO2" t="n">
-        <v>2.073339243026685e-85</v>
+        <v>1.001307404362106e-68</v>
       </c>
       <c r="AP2" t="n">
-        <v>3.338661241582583e-89</v>
+        <v>1.119464915400031e-71</v>
       </c>
       <c r="AQ2" t="n">
-        <v>4.605903120284236e-93</v>
+        <v>2.109487073299156e-73</v>
       </c>
       <c r="AR2" t="n">
-        <v>2.772173082594918e-97</v>
+        <v>4.66895425764985e-76</v>
       </c>
       <c r="AS2" t="n">
-        <v>4.461252388693925e-101</v>
+        <v>2.212267169697267e-78</v>
       </c>
       <c r="AT2" t="n">
-        <v>3.442905348357114e-105</v>
+        <v>8.153553115157176e-81</v>
       </c>
       <c r="AU2" t="n">
-        <v>4.937621130350843e-109</v>
+        <v>2.071135538019911e-83</v>
       </c>
       <c r="AV2" t="n">
-        <v>1.562808955496047e-112</v>
+        <v>8.064941045326629e-86</v>
       </c>
       <c r="AW2" t="n">
-        <v>1.046762319410055e-116</v>
+        <v>1.757044808891067e-88</v>
       </c>
       <c r="AX2" t="n">
-        <v>1.718983701685565e-120</v>
+        <v>5.168908558475234e-91</v>
       </c>
       <c r="AY2" t="n">
-        <v>3.057106711757693e-124</v>
+        <v>9.148877861852233e-94</v>
       </c>
       <c r="AZ2" t="n">
-        <v>2.856138941436403e-128</v>
+        <v>1.871023246356818e-96</v>
       </c>
       <c r="BA2" t="n">
-        <v>2.810901436987824e-132</v>
+        <v>2.690422145843421e-99</v>
       </c>
       <c r="BB2" t="n">
-        <v>3.234235492614173e-136</v>
+        <v>7.761835446567917e-102</v>
       </c>
       <c r="BC2" t="n">
-        <v>2.211776960842296e-140</v>
+        <v>6.217801520294751e-104</v>
       </c>
       <c r="BD2" t="n">
-        <v>9.607945606298793e-145</v>
+        <v>7.122701642586509e-106</v>
       </c>
       <c r="BE2" t="n">
-        <v>9.242227697721345e-149</v>
+        <v>1.946831423840456e-108</v>
       </c>
       <c r="BF2" t="n">
-        <v>4.74204472904322e-153</v>
+        <v>2.116078230656385e-111</v>
       </c>
       <c r="BG2" t="n">
-        <v>2.492861391574399e-157</v>
+        <v>6.474145173102189e-114</v>
       </c>
       <c r="BH2" t="n">
-        <v>5.92084112844013e-162</v>
+        <v>9.440426568378082e-117</v>
       </c>
       <c r="BI2" t="n">
-        <v>2.061798567574792e-166</v>
+        <v>2.755214100351078e-119</v>
       </c>
       <c r="BJ2" t="n">
-        <v>1.067246492393343e-170</v>
+        <v>3.674283170389073e-122</v>
       </c>
       <c r="BK2" t="n">
-        <v>2.715061396828619e-175</v>
+        <v>1.438685671696108e-124</v>
       </c>
       <c r="BL2" t="n">
-        <v>5.255281453179585e-180</v>
+        <v>6.506268670422225e-127</v>
       </c>
       <c r="BM2" t="n">
-        <v>1.818283227712828e-184</v>
+        <v>9.919357392084052e-130</v>
       </c>
       <c r="BN2" t="n">
-        <v>7.193145057543902e-189</v>
+        <v>2.410274017315642e-132</v>
       </c>
       <c r="BO2" t="n">
-        <v>9.630541537454696e-194</v>
+        <v>3.944102060422924e-135</v>
       </c>
       <c r="BP2" t="n">
-        <v>4.976593841372967e-198</v>
+        <v>6.182541622744581e-138</v>
       </c>
       <c r="BQ2" t="n">
-        <v>1.277222745672072e-202</v>
+        <v>3.978848303220682e-140</v>
       </c>
       <c r="BR2" t="n">
-        <v>3.950911502274632e-207</v>
+        <v>8.691316727128241e-143</v>
       </c>
       <c r="BS2" t="n">
-        <v>7.817056697722441e-212</v>
+        <v>1.365489556965268e-145</v>
       </c>
       <c r="BT2" t="n">
-        <v>1.115285760267301e-215</v>
+        <v>4.294932470155662e-148</v>
       </c>
       <c r="BU2" t="n">
-        <v>2.714982372939009e-220</v>
+        <v>6.034930256155181e-151</v>
       </c>
       <c r="BV2" t="n">
-        <v>8.359522876826865e-225</v>
+        <v>2.746389095957429e-153</v>
       </c>
       <c r="BW2" t="n">
-        <v>1.297501904423602e-229</v>
+        <v>3.171583453470625e-156</v>
       </c>
       <c r="BX2" t="n">
-        <v>2.678530801934219e-234</v>
+        <v>2.440346018088002e-158</v>
       </c>
       <c r="BY2" t="n">
-        <v>1.431194226257497e-238</v>
+        <v>3.544556537454482e-161</v>
       </c>
       <c r="BZ2" t="n">
-        <v>3.845742873247014e-243</v>
+        <v>6.107568650695638e-164</v>
       </c>
       <c r="CA2" t="n">
-        <v>9.232076984674045e-248</v>
+        <v>1.253677662089693e-166</v>
       </c>
       <c r="CB2" t="n">
-        <v>3.970720153543433e-252</v>
+        <v>9.684158578974107e-170</v>
       </c>
       <c r="CC2" t="n">
-        <v>7.491506742692672e-257</v>
+        <v>1.32209818170227e-172</v>
       </c>
       <c r="CD2" t="n">
-        <v>3.948025945351771e-261</v>
+        <v>2.783491390160508e-175</v>
       </c>
       <c r="CE2" t="n">
-        <v>8.524626524707715e-266</v>
+        <v>1.800091067006812e-178</v>
       </c>
       <c r="CF2" t="n">
-        <v>6.299957774818887e-270</v>
+        <v>9.416852321454687e-182</v>
       </c>
       <c r="CG2" t="n">
-        <v>1.173966501515781e-274</v>
+        <v>1.676920949558566e-184</v>
       </c>
       <c r="CH2" t="n">
-        <v>3.617109981685901e-279</v>
+        <v>3.686377533057481e-187</v>
       </c>
       <c r="CI2" t="n">
-        <v>2.257222626181034e-283</v>
+        <v>8.243070229873202e-190</v>
       </c>
       <c r="CJ2" t="n">
-        <v>4.021236841108703e-288</v>
+        <v>8.117517979144395e-193</v>
       </c>
       <c r="CK2" t="n">
-        <v>7.59863102319248e-293</v>
+        <v>5.900691178319748e-196</v>
       </c>
       <c r="CL2" t="n">
-        <v>7.728367113550322e-298</v>
+        <v>4.700291342577031e-199</v>
       </c>
       <c r="CM2" t="n">
-        <v>3.863538316039096e-302</v>
+        <v>3.915608420518692e-202</v>
       </c>
       <c r="CN2" t="n">
-        <v>6.536786278814825e-307</v>
+        <v>3.507653460810378e-205</v>
       </c>
       <c r="CO2" t="n">
-        <v>0</v>
+        <v>4.163272424767511e-208</v>
       </c>
       <c r="CP2" t="n">
-        <v>0</v>
+        <v>6.170972891235018e-211</v>
       </c>
       <c r="CQ2" t="n">
-        <v>0</v>
+        <v>1.722416482983059e-213</v>
       </c>
       <c r="CR2" t="n">
-        <v>0</v>
+        <v>2.973626313121827e-216</v>
       </c>
       <c r="CS2" t="n">
-        <v>0</v>
+        <v>6.128449823203112e-219</v>
       </c>
       <c r="CT2" t="n">
-        <v>0</v>
+        <v>3.219433825610468e-222</v>
       </c>
       <c r="CU2" t="n">
-        <v>0</v>
+        <v>2.169453561257874e-225</v>
       </c>
       <c r="CV2" t="n">
-        <v>0</v>
+        <v>1.622958145967676e-228</v>
       </c>
       <c r="CW2" t="n">
-        <v>0</v>
+        <v>1.676519465183634e-231</v>
       </c>
       <c r="CX2" t="n">
-        <v>0</v>
+        <v>2.537791476351812e-234</v>
       </c>
       <c r="CY2" t="n">
-        <v>0</v>
+        <v>2.836855896989949e-237</v>
       </c>
       <c r="CZ2" t="n">
-        <v>0</v>
+        <v>1.76348113165736e-240</v>
       </c>
       <c r="DA2" t="n">
-        <v>0</v>
+        <v>1.255249483682993e-243</v>
       </c>
       <c r="DB2" t="n">
-        <v>0</v>
+        <v>1.081978326625787e-246</v>
       </c>
       <c r="DC2" t="n">
-        <v>0</v>
+        <v>9.655965717845668e-250</v>
       </c>
       <c r="DD2" t="n">
-        <v>0</v>
+        <v>6.602105571251329e-253</v>
       </c>
       <c r="DE2" t="n">
-        <v>0</v>
+        <v>6.813791156516597e-256</v>
       </c>
       <c r="DF2" t="n">
-        <v>0</v>
+        <v>6.497225314451537e-259</v>
       </c>
       <c r="DG2" t="n">
-        <v>0</v>
+        <v>3.654544185253556e-262</v>
       </c>
       <c r="DH2" t="n">
-        <v>0</v>
+        <v>5.117197616000626e-265</v>
       </c>
       <c r="DI2" t="n">
-        <v>0</v>
+        <v>5.559351025347052e-268</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0</v>
+        <v>5.41051838730642e-270</v>
       </c>
       <c r="DK2" t="n">
-        <v>0</v>
+        <v>3.131376594283179e-272</v>
       </c>
       <c r="DL2" t="n">
-        <v>0</v>
+        <v>7.573765947204086e-275</v>
       </c>
       <c r="DM2" t="n">
-        <v>0</v>
+        <v>4.292768659784563e-278</v>
       </c>
       <c r="DN2" t="n">
-        <v>0</v>
+        <v>2.901252330862475e-280</v>
       </c>
       <c r="DO2" t="n">
-        <v>0</v>
+        <v>1.598709069917654e-283</v>
       </c>
       <c r="DP2" t="n">
-        <v>0</v>
+        <v>2.433169690280354e-286</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0</v>
+        <v>8.850241902275137e-289</v>
       </c>
       <c r="DR2" t="n">
-        <v>0</v>
+        <v>7.288965620203815e-292</v>
       </c>
       <c r="DS2" t="n">
-        <v>0</v>
+        <v>7.657739693360492e-295</v>
       </c>
       <c r="DT2" t="n">
-        <v>0</v>
+        <v>7.845714569900827e-298</v>
       </c>
       <c r="DU2" t="n">
-        <v>0</v>
+        <v>1.877631042530175e-299</v>
       </c>
       <c r="DV2" t="n">
-        <v>0</v>
+        <v>1.474720506474386e-302</v>
       </c>
       <c r="DW2" t="n">
-        <v>0</v>
+        <v>1.27006762243791e-305</v>
       </c>
       <c r="DX2" t="n">
-        <v>0</v>
+        <v>1.536564190134748e-308</v>
       </c>
       <c r="DY2" t="n">
         <v>0</v>
@@ -15535,436 +15535,436 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3348059421823459</v>
+        <v>0.3218967437036799</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3362775666729259</v>
+        <v>0.3109195809270577</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3362775666729259</v>
+        <v>0.3109195809270577</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3387574288129209</v>
+        <v>0.3145586285388154</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3469950499379489</v>
+        <v>0.3337435446759404</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3280180686999355</v>
+        <v>0.2349293503472671</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3362999164551781</v>
+        <v>0.1318954884372889</v>
       </c>
       <c r="I3" t="n">
-        <v>0.428683788708678</v>
+        <v>0.0334361747550254</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5091284863449616</v>
+        <v>0.006713518611122396</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3782409312938019</v>
+        <v>0.00149657927312792</v>
       </c>
       <c r="L3" t="n">
-        <v>0.4929459822486369</v>
+        <v>0.0002167091615236366</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1726707998399122</v>
+        <v>2.321900751363524e-05</v>
       </c>
       <c r="N3" t="n">
-        <v>0.04784603541018313</v>
+        <v>3.095508295378558e-06</v>
       </c>
       <c r="O3" t="n">
-        <v>0.01466296819738681</v>
+        <v>1.034972811416586e-06</v>
       </c>
       <c r="P3" t="n">
-        <v>0.002240120002980254</v>
+        <v>2.284798667421299e-07</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0007484062754188388</v>
+        <v>1.682184684508217e-08</v>
       </c>
       <c r="R3" t="n">
-        <v>5.265837945289228e-05</v>
+        <v>6.286462781141085e-10</v>
       </c>
       <c r="S3" t="n">
-        <v>4.875999026495123e-06</v>
+        <v>6.900138074965985e-11</v>
       </c>
       <c r="T3" t="n">
-        <v>3.930011248059979e-06</v>
+        <v>1.307415775395579e-12</v>
       </c>
       <c r="U3" t="n">
-        <v>3.752519988905894e-07</v>
+        <v>5.262344230934266e-13</v>
       </c>
       <c r="V3" t="n">
-        <v>2.584478143256806e-08</v>
+        <v>5.486280787489347e-15</v>
       </c>
       <c r="W3" t="n">
-        <v>8.892861424272279e-10</v>
+        <v>2.498050803560655e-16</v>
       </c>
       <c r="X3" t="n">
-        <v>3.904565025834886e-11</v>
+        <v>8.064512165139064e-18</v>
       </c>
       <c r="Y3" t="n">
-        <v>3.751366046176186e-11</v>
+        <v>1.564386188292091e-19</v>
       </c>
       <c r="Z3" t="n">
-        <v>5.258425940414895e-13</v>
+        <v>6.166022420355591e-21</v>
       </c>
       <c r="AA3" t="n">
-        <v>2.391583039619113e-15</v>
+        <v>5.070431138621706e-23</v>
       </c>
       <c r="AB3" t="n">
-        <v>3.797696020079955e-17</v>
+        <v>2.112601166772899e-24</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.275111618755141e-19</v>
+        <v>1.068655754182015e-25</v>
       </c>
       <c r="AD3" t="n">
-        <v>8.097552375637875e-22</v>
+        <v>2.132797225464027e-27</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.581750768660109e-24</v>
+        <v>2.712510334143852e-29</v>
       </c>
       <c r="AF3" t="n">
-        <v>8.59926889724044e-27</v>
+        <v>9.707062441061578e-31</v>
       </c>
       <c r="AG3" t="n">
-        <v>1.756837898326819e-29</v>
+        <v>4.130882805256989e-32</v>
       </c>
       <c r="AH3" t="n">
-        <v>1.25263470719974e-31</v>
+        <v>6.846080431471238e-33</v>
       </c>
       <c r="AI3" t="n">
-        <v>5.554540084140055e-34</v>
+        <v>3.84414223625198e-34</v>
       </c>
       <c r="AJ3" t="n">
-        <v>5.705532091185654e-36</v>
+        <v>1.410240425706752e-35</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.37055317795475e-38</v>
+        <v>1.74080716871126e-37</v>
       </c>
       <c r="AL3" t="n">
-        <v>9.856327374423091e-41</v>
+        <v>7.42357692007471e-40</v>
       </c>
       <c r="AM3" t="n">
-        <v>2.432572907261946e-42</v>
+        <v>1.402242855471171e-42</v>
       </c>
       <c r="AN3" t="n">
-        <v>3.090757358346238e-44</v>
+        <v>6.188480341468662e-45</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.171288426218854e-47</v>
+        <v>6.621538494919898e-48</v>
       </c>
       <c r="AP3" t="n">
-        <v>2.536571722266149e-50</v>
+        <v>8.933725142367882e-51</v>
       </c>
       <c r="AQ3" t="n">
-        <v>3.726917907351445e-53</v>
+        <v>4.05298489716553e-52</v>
       </c>
       <c r="AR3" t="n">
-        <v>3.400181461335707e-56</v>
+        <v>1.602815489825528e-54</v>
       </c>
       <c r="AS3" t="n">
-        <v>1.059445562560531e-58</v>
+        <v>9.374059712641047e-57</v>
       </c>
       <c r="AT3" t="n">
-        <v>5.998166238168e-62</v>
+        <v>6.327452601776492e-59</v>
       </c>
       <c r="AU3" t="n">
-        <v>8.537313079795589e-65</v>
+        <v>2.975365452267407e-61</v>
       </c>
       <c r="AV3" t="n">
-        <v>1.930496912463523e-67</v>
+        <v>3.427760444770435e-63</v>
       </c>
       <c r="AW3" t="n">
-        <v>1.789546963355051e-70</v>
+        <v>2.181069037315696e-65</v>
       </c>
       <c r="AX3" t="n">
-        <v>5.052704275384854e-73</v>
+        <v>2.061704828531592e-67</v>
       </c>
       <c r="AY3" t="n">
-        <v>6.648999867263267e-76</v>
+        <v>9.51586597136562e-70</v>
       </c>
       <c r="AZ3" t="n">
-        <v>6.709223675204035e-79</v>
+        <v>2.082765914230343e-72</v>
       </c>
       <c r="BA3" t="n">
-        <v>6.582609208701772e-82</v>
+        <v>6.091384758318366e-75</v>
       </c>
       <c r="BB3" t="n">
-        <v>8.110923263169645e-85</v>
+        <v>3.866532065390961e-77</v>
       </c>
       <c r="BC3" t="n">
-        <v>3.215572862616799e-88</v>
+        <v>8.975632722643542e-79</v>
       </c>
       <c r="BD3" t="n">
-        <v>1.326022156603906e-91</v>
+        <v>3.044771333386425e-80</v>
       </c>
       <c r="BE3" t="n">
-        <v>1.55899510779364e-94</v>
+        <v>1.760817731412544e-82</v>
       </c>
       <c r="BF3" t="n">
-        <v>6.023128091436957e-98</v>
+        <v>3.404015359284273e-85</v>
       </c>
       <c r="BG3" t="n">
-        <v>3.022411389503915e-101</v>
+        <v>3.48887080525409e-87</v>
       </c>
       <c r="BH3" t="n">
-        <v>3.551371251865455e-105</v>
+        <v>1.217304413826287e-89</v>
       </c>
       <c r="BI3" t="n">
-        <v>8.779923643196093e-109</v>
+        <v>7.684645912527005e-92</v>
       </c>
       <c r="BJ3" t="n">
-        <v>3.470264652913819e-112</v>
+        <v>2.232521334768168e-94</v>
       </c>
       <c r="BK3" t="n">
-        <v>4.21713671115612e-116</v>
+        <v>1.622261075859878e-96</v>
       </c>
       <c r="BL3" t="n">
-        <v>3.884121666106126e-120</v>
+        <v>1.974581690474197e-98</v>
       </c>
       <c r="BM3" t="n">
-        <v>5.817585040250719e-124</v>
+        <v>4.817764277499923e-101</v>
       </c>
       <c r="BN3" t="n">
-        <v>1.121946544310472e-127</v>
+        <v>2.567194675804807e-103</v>
       </c>
       <c r="BO3" t="n">
-        <v>4.252273406871289e-132</v>
+        <v>1.180924255997946e-105</v>
       </c>
       <c r="BP3" t="n">
-        <v>5.944269914493058e-136</v>
+        <v>5.105850393792901e-108</v>
       </c>
       <c r="BQ3" t="n">
-        <v>7.812597965996317e-140</v>
+        <v>8.290336373680766e-110</v>
       </c>
       <c r="BR3" t="n">
-        <v>1.286506546823796e-143</v>
+        <v>5.667044733495983e-112</v>
       </c>
       <c r="BS3" t="n">
-        <v>8.749519790401353e-148</v>
+        <v>1.357670702954814e-114</v>
       </c>
       <c r="BT3" t="n">
-        <v>4.421591667581144e-151</v>
+        <v>1.154809841221137e-116</v>
       </c>
       <c r="BU3" t="n">
-        <v>3.054532075220023e-155</v>
+        <v>3.87514065956852e-119</v>
       </c>
       <c r="BV3" t="n">
-        <v>4.36658606275486e-159</v>
+        <v>3.398228386753844e-121</v>
       </c>
       <c r="BW3" t="n">
-        <v>2.301675843751733e-163</v>
+        <v>7.586295154269544e-124</v>
       </c>
       <c r="BX3" t="n">
-        <v>1.884600810924702e-167</v>
+        <v>1.864915771608332e-125</v>
       </c>
       <c r="BY3" t="n">
-        <v>6.521880163493172e-171</v>
+        <v>5.355736901956821e-128</v>
       </c>
       <c r="BZ3" t="n">
-        <v>6.113058328251727e-175</v>
+        <v>1.835972356878069e-130</v>
       </c>
       <c r="CA3" t="n">
-        <v>3.723593532736485e-179</v>
+        <v>8.057187406247473e-133</v>
       </c>
       <c r="CB3" t="n">
-        <v>9.617810444791699e-183</v>
+        <v>9.243411118597292e-136</v>
       </c>
       <c r="CC3" t="n">
-        <v>5.93614554387477e-187</v>
+        <v>2.602259464763891e-138</v>
       </c>
       <c r="CD3" t="n">
-        <v>1.570118072871645e-190</v>
+        <v>1.401103296895474e-140</v>
       </c>
       <c r="CE3" t="n">
-        <v>1.16831315687021e-194</v>
+        <v>1.007280672719275e-143</v>
       </c>
       <c r="CF3" t="n">
-        <v>3.65892263492056e-198</v>
+        <v>3.144687485896004e-147</v>
       </c>
       <c r="CG3" t="n">
-        <v>1.980330160344301e-202</v>
+        <v>1.132533131918807e-149</v>
       </c>
       <c r="CH3" t="n">
-        <v>2.959821413297728e-206</v>
+        <v>7.012074645130917e-152</v>
       </c>
       <c r="CI3" t="n">
-        <v>4.793595170346115e-210</v>
+        <v>4.106289387217895e-154</v>
       </c>
       <c r="CJ3" t="n">
-        <v>2.159087530346648e-214</v>
+        <v>7.340806285885772e-157</v>
       </c>
       <c r="CK3" t="n">
-        <v>1.481935116668392e-218</v>
+        <v>8.738786946627308e-160</v>
       </c>
       <c r="CL3" t="n">
-        <v>3.239978438901974e-223</v>
+        <v>1.346993083060096e-162</v>
       </c>
       <c r="CM3" t="n">
-        <v>6.285770243079764e-227</v>
+        <v>2.29112986525448e-165</v>
       </c>
       <c r="CN3" t="n">
-        <v>2.618716705745041e-231</v>
+        <v>4.34546368086057e-168</v>
       </c>
       <c r="CO3" t="n">
-        <v>8.657925580087935e-236</v>
+        <v>1.150162461851817e-170</v>
       </c>
       <c r="CP3" t="n">
-        <v>6.26063709916858e-240</v>
+        <v>3.30777992576676e-173</v>
       </c>
       <c r="CQ3" t="n">
-        <v>7.817167660378272e-244</v>
+        <v>2.779692619701591e-175</v>
       </c>
       <c r="CR3" t="n">
-        <v>1.679050535825766e-247</v>
+        <v>1.436444715234375e-177</v>
       </c>
       <c r="CS3" t="n">
-        <v>1.479521798477182e-251</v>
+        <v>1.54022701243066e-180</v>
       </c>
       <c r="CT3" t="n">
-        <v>2.235216412717933e-255</v>
+        <v>2.996717533198303e-184</v>
       </c>
       <c r="CU3" t="n">
-        <v>4.138271521969739e-259</v>
+        <v>2.680501960070904e-187</v>
       </c>
       <c r="CV3" t="n">
-        <v>2.849026237656208e-263</v>
+        <v>3.918924806759482e-190</v>
       </c>
       <c r="CW3" t="n">
-        <v>1.45127923817932e-267</v>
+        <v>9.265850491755554e-193</v>
       </c>
       <c r="CX3" t="n">
-        <v>7.741975459817909e-273</v>
+        <v>2.186336870585235e-195</v>
       </c>
       <c r="CY3" t="n">
-        <v>7.029234828690417e-278</v>
+        <v>3.415152328137417e-198</v>
       </c>
       <c r="CZ3" t="n">
-        <v>1.803431396358626e-281</v>
+        <v>1.418521274984446e-201</v>
       </c>
       <c r="DA3" t="n">
-        <v>6.793661921116403e-286</v>
+        <v>9.926940974410778e-205</v>
       </c>
       <c r="DB3" t="n">
-        <v>1.04992275848699e-289</v>
+        <v>9.74000343156007e-208</v>
       </c>
       <c r="DC3" t="n">
-        <v>7.767299543129714e-294</v>
+        <v>2.09129406068677e-210</v>
       </c>
       <c r="DD3" t="n">
-        <v>1.059255849574217e-298</v>
+        <v>2.601931542739223e-213</v>
       </c>
       <c r="DE3" t="n">
-        <v>8.777049757305291e-303</v>
+        <v>5.286210085154298e-216</v>
       </c>
       <c r="DF3" t="n">
-        <v>3.628618993839384e-307</v>
+        <v>6.315799202148491e-219</v>
       </c>
       <c r="DG3" t="n">
-        <v>0</v>
+        <v>3.88870067303608e-222</v>
       </c>
       <c r="DH3" t="n">
-        <v>0</v>
+        <v>9.02310341055562e-225</v>
       </c>
       <c r="DI3" t="n">
-        <v>0</v>
+        <v>1.829385383053197e-227</v>
       </c>
       <c r="DJ3" t="n">
-        <v>0</v>
+        <v>4.773149859876093e-229</v>
       </c>
       <c r="DK3" t="n">
-        <v>0</v>
+        <v>6.93176756531318e-231</v>
       </c>
       <c r="DL3" t="n">
-        <v>0</v>
+        <v>3.611040247312697e-233</v>
       </c>
       <c r="DM3" t="n">
-        <v>0</v>
+        <v>2.29976780567322e-236</v>
       </c>
       <c r="DN3" t="n">
-        <v>0</v>
+        <v>6.542056515799886e-238</v>
       </c>
       <c r="DO3" t="n">
-        <v>0</v>
+        <v>2.993802795723802e-241</v>
       </c>
       <c r="DP3" t="n">
-        <v>0</v>
+        <v>8.167609769668029e-244</v>
       </c>
       <c r="DQ3" t="n">
-        <v>0</v>
+        <v>7.068205604888672e-246</v>
       </c>
       <c r="DR3" t="n">
-        <v>0</v>
+        <v>8.769799978862183e-249</v>
       </c>
       <c r="DS3" t="n">
-        <v>0</v>
+        <v>2.290032585477376e-251</v>
       </c>
       <c r="DT3" t="n">
-        <v>0</v>
+        <v>3.735221479643302e-254</v>
       </c>
       <c r="DU3" t="n">
-        <v>0</v>
+        <v>1.582958883957275e-255</v>
       </c>
       <c r="DV3" t="n">
-        <v>0</v>
+        <v>1.911821881237306e-258</v>
       </c>
       <c r="DW3" t="n">
-        <v>0</v>
+        <v>3.9911161750475e-261</v>
       </c>
       <c r="DX3" t="n">
-        <v>0</v>
+        <v>1.368664386267611e-263</v>
       </c>
       <c r="DY3" t="n">
-        <v>0</v>
+        <v>3.40159899273117e-266</v>
       </c>
       <c r="DZ3" t="n">
-        <v>0</v>
+        <v>2.512669810605646e-269</v>
       </c>
       <c r="EA3" t="n">
-        <v>0</v>
+        <v>1.515912910076577e-271</v>
       </c>
       <c r="EB3" t="n">
-        <v>0</v>
+        <v>1.099898404403675e-273</v>
       </c>
       <c r="EC3" t="n">
-        <v>0</v>
+        <v>3.237148554620284e-276</v>
       </c>
       <c r="ED3" t="n">
-        <v>0</v>
+        <v>9.430612239309615e-278</v>
       </c>
       <c r="EE3" t="n">
-        <v>0</v>
+        <v>2.57778564696877e-280</v>
       </c>
       <c r="EF3" t="n">
-        <v>0</v>
+        <v>4.393089312715221e-283</v>
       </c>
       <c r="EG3" t="n">
-        <v>0</v>
+        <v>8.518586153834507e-286</v>
       </c>
       <c r="EH3" t="n">
-        <v>0</v>
+        <v>2.984532057077261e-288</v>
       </c>
       <c r="EI3" t="n">
-        <v>0</v>
+        <v>3.442472960843656e-291</v>
       </c>
       <c r="EJ3" t="n">
-        <v>0</v>
+        <v>5.802668315861809e-294</v>
       </c>
       <c r="EK3" t="n">
-        <v>0</v>
+        <v>1.202348892314289e-296</v>
       </c>
       <c r="EL3" t="n">
-        <v>0</v>
+        <v>1.909605465558313e-299</v>
       </c>
       <c r="EM3" t="n">
-        <v>0</v>
+        <v>3.525737051175002e-302</v>
       </c>
       <c r="EN3" t="n">
-        <v>0</v>
+        <v>9.000778007935077e-305</v>
       </c>
       <c r="EO3" t="n">
-        <v>0</v>
+        <v>1.245504882239278e-307</v>
       </c>
       <c r="EP3" t="n">
         <v>0</v>
@@ -17042,82 +17042,82 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3303891211769477</v>
+        <v>0.3561987022373505</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3274468857836201</v>
+        <v>0.3781466331410824</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3274468857836201</v>
+        <v>0.3781466331410824</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3225104512257225</v>
+        <v>0.3934804273656909</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3653886425344118</v>
+        <v>0.3863599599663047</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4933794565699353</v>
+        <v>0.6888993249717745</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5418176968671548</v>
+        <v>0.8515045542911349</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4159788147210483</v>
+        <v>0.9650815492974342</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3811111002632885</v>
+        <v>0.993235662052482</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6008546193486469</v>
+        <v>0.9985005672608062</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4953690230178424</v>
+        <v>0.9997831588243581</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8267945468820297</v>
+        <v>0.9999767780710369</v>
       </c>
       <c r="N4" t="n">
-        <v>0.952120981429646</v>
+        <v>0.9999969044183361</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9853361745566372</v>
+        <v>0.9999989650252694</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9977598696845874</v>
+        <v>0.9999997715200333</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9992515934295433</v>
+        <v>0.9999999831781518</v>
       </c>
       <c r="R4" t="n">
-        <v>0.999947341618194</v>
+        <v>0.9999999993713538</v>
       </c>
       <c r="S4" t="n">
-        <v>0.9999951240009654</v>
+        <v>0.9999999999309985</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9999960699887518</v>
+        <v>0.9999999999986925</v>
       </c>
       <c r="U4" t="n">
-        <v>0.999999624748001</v>
+        <v>0.9999999999994736</v>
       </c>
       <c r="V4" t="n">
-        <v>0.9999999741552186</v>
+        <v>0.9999999999999944</v>
       </c>
       <c r="W4" t="n">
-        <v>0.9999999991107139</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="X4" t="n">
-        <v>0.9999999999609543</v>
+        <v>1</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.9999999999624863</v>
+        <v>1</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.9999999999994741</v>
+        <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.9999999999999977</v>
+        <v>1</v>
       </c>
       <c r="AB4" t="n">
         <v>1</v>

</xml_diff>